<commit_message>
updating generate electric field tables with decay
</commit_message>
<xml_diff>
--- a/util/icecube_acceptance.xlsx
+++ b/util/icecube_acceptance.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31000" yWindow="10200" windowWidth="24160" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="1180" windowWidth="24160" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="icecube_acceptance.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -531,7 +531,7 @@
         <v>11.979551673969199</v>
       </c>
       <c r="C3">
-        <f>POWER(10, B3-10)/$N$3</f>
+        <f t="shared" ref="C3:C34" si="0">POWER(10, B3-10)/$N$3</f>
         <v>4.5514223201753288E-7</v>
       </c>
       <c r="D3">
@@ -541,7 +541,7 @@
         <v>12.020664990976</v>
       </c>
       <c r="F3">
-        <f>POWER(10, E3-10)/$N$3</f>
+        <f t="shared" ref="F3:F34" si="1">POWER(10, E3-10)/$N$3</f>
         <v>5.0033450203391288E-7</v>
       </c>
       <c r="G3">
@@ -551,7 +551,7 @@
         <v>12.013846700824001</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="0">POWER(10, H3-10)/$N$3</f>
+        <f t="shared" ref="I3:I66" si="2">POWER(10, H3-10)/$N$3</f>
         <v>4.9254074371361153E-7</v>
       </c>
       <c r="J3">
@@ -561,7 +561,7 @@
         <v>12.023877872285</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L66" si="1">POWER(10, K3-10)/$N$3</f>
+        <f t="shared" ref="L3:L66" si="3">POWER(10, K3-10)/$N$3</f>
         <v>5.0404966829199579E-7</v>
       </c>
       <c r="M3">
@@ -579,7 +579,7 @@
         <v>12.3116347673402</v>
       </c>
       <c r="C4">
-        <f>POWER(10, B4-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>9.777554116059838E-7</v>
       </c>
       <c r="D4">
@@ -589,7 +589,7 @@
         <v>12.3339875579512</v>
       </c>
       <c r="F4">
-        <f>POWER(10, E4-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.0293972860971493E-6</v>
       </c>
       <c r="G4">
@@ -599,7 +599,7 @@
         <v>12.104843423721601</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0734978867375655E-7</v>
       </c>
       <c r="J4">
@@ -609,7 +609,7 @@
         <v>12.112287538826299</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.1784992716697401E-7</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -624,7 +624,7 @@
         <v>12.195446336726199</v>
       </c>
       <c r="C5">
-        <f>POWER(10, B5-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>7.4824150990353195E-7</v>
       </c>
       <c r="D5">
@@ -634,7 +634,7 @@
         <v>12.208767664360799</v>
       </c>
       <c r="F5">
-        <f>POWER(10, E5-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>7.7154831183309275E-7</v>
       </c>
       <c r="G5">
@@ -644,7 +644,7 @@
         <v>12.199177688552099</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5469791390990651E-7</v>
       </c>
       <c r="J5">
@@ -654,7 +654,7 @@
         <v>12.1934824667513</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4486561706870449E-7</v>
       </c>
     </row>
@@ -666,7 +666,7 @@
         <v>12.118307815306601</v>
       </c>
       <c r="C6">
-        <f>POWER(10, B6-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>6.2647432418291061E-7</v>
       </c>
       <c r="D6">
@@ -676,7 +676,7 @@
         <v>12.4340361389494</v>
       </c>
       <c r="F6">
-        <f>POWER(10, E6-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.2960793760695447E-6</v>
       </c>
       <c r="G6">
@@ -686,7 +686,7 @@
         <v>12.2874786219946</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.2485592460533784E-7</v>
       </c>
       <c r="J6">
@@ -696,7 +696,7 @@
         <v>12.277680993867</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.042248847074522E-7</v>
       </c>
     </row>
@@ -708,7 +708,7 @@
         <v>12.037161848442199</v>
       </c>
       <c r="C7">
-        <f>POWER(10, B7-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>5.1970549579163583E-7</v>
       </c>
       <c r="D7">
@@ -718,7 +718,7 @@
         <v>12.5122413616345</v>
       </c>
       <c r="F7">
-        <f>POWER(10, E7-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.551803841474921E-6</v>
       </c>
       <c r="G7">
@@ -728,7 +728,7 @@
         <v>12.369784378528101</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1178404979833432E-6</v>
       </c>
       <c r="J7">
@@ -738,7 +738,7 @@
         <v>12.3703933908424</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.119409148309624E-6</v>
       </c>
     </row>
@@ -750,7 +750,7 @@
         <v>11.966119912668701</v>
       </c>
       <c r="C8">
-        <f>POWER(10, B8-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>4.4128114732730155E-7</v>
       </c>
       <c r="D8">
@@ -760,7 +760,7 @@
         <v>12.5950839083325</v>
       </c>
       <c r="F8">
-        <f>POWER(10, E8-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.8779298679201243E-6</v>
       </c>
       <c r="G8">
@@ -770,7 +770,7 @@
         <v>12.451919040955699</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3505619250189747E-6</v>
       </c>
       <c r="J8">
@@ -780,7 +780,7 @@
         <v>12.455969552247799</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3632170625017857E-6</v>
       </c>
     </row>
@@ -792,7 +792,7 @@
         <v>12.436323171848599</v>
       </c>
       <c r="C9">
-        <f>POWER(10, B9-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.3029226467563407E-6</v>
       </c>
       <c r="D9">
@@ -802,7 +802,7 @@
         <v>12.683446323462199</v>
       </c>
       <c r="F9">
-        <f>POWER(10, E9-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.3016632549748102E-6</v>
       </c>
       <c r="G9">
@@ -812,7 +812,7 @@
         <v>12.5345990728551</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.6337836059043367E-6</v>
       </c>
       <c r="J9">
@@ -822,7 +822,7 @@
         <v>12.5365986066553</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6413230464861584E-6</v>
       </c>
     </row>
@@ -834,7 +834,7 @@
         <v>12.5335254495035</v>
       </c>
       <c r="C10">
-        <f>POWER(10, B10-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.6297497027229012E-6</v>
       </c>
       <c r="D10">
@@ -844,7 +844,7 @@
         <v>12.7705763420811</v>
       </c>
       <c r="F10">
-        <f>POWER(10, E10-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.8130134136489863E-6</v>
       </c>
       <c r="G10">
@@ -854,7 +854,7 @@
         <v>12.6260825737084</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0168705972401809E-6</v>
       </c>
       <c r="J10">
@@ -864,7 +864,7 @@
         <v>12.619607193385599</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9870219029967818E-6</v>
       </c>
     </row>
@@ -876,7 +876,7 @@
         <v>12.6363854378368</v>
       </c>
       <c r="C11">
-        <f>POWER(10, B11-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.0652893181024261E-6</v>
       </c>
       <c r="D11">
@@ -886,7 +886,7 @@
         <v>12.856750915327</v>
       </c>
       <c r="F11">
-        <f>POWER(10, E11-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.4304127379320456E-6</v>
       </c>
       <c r="G11">
@@ -896,7 +896,7 @@
         <v>12.7027318824865</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4061757384654503E-6</v>
       </c>
       <c r="J11">
@@ -906,7 +906,7 @@
         <v>12.7018387936014</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.4012327312016271E-6</v>
       </c>
     </row>
@@ -918,7 +918,7 @@
         <v>12.744235340094001</v>
       </c>
       <c r="C12">
-        <f>POWER(10, B12-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.6474684974329554E-6</v>
       </c>
       <c r="D12">
@@ -928,7 +928,7 @@
         <v>12.9438198665905</v>
       </c>
       <c r="F12">
-        <f>POWER(10, E12-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>4.1919426031952488E-6</v>
       </c>
       <c r="G12">
@@ -938,7 +938,7 @@
         <v>12.7898134756384</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.940417079037278E-6</v>
       </c>
       <c r="J12">
@@ -948,7 +948,7 @@
         <v>12.781368887970499</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8837947639929699E-6</v>
       </c>
     </row>
@@ -960,7 +960,7 @@
         <v>12.830710967669599</v>
       </c>
       <c r="C13">
-        <f>POWER(10, B13-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.2307728801741338E-6</v>
       </c>
       <c r="D13">
@@ -970,7 +970,7 @@
         <v>13.028958686460401</v>
       </c>
       <c r="F13">
-        <f>POWER(10, E13-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>5.0998117761230631E-6</v>
       </c>
       <c r="G13">
@@ -980,7 +980,7 @@
         <v>12.8818301312457</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6343403198349643E-6</v>
       </c>
       <c r="J13">
@@ -990,7 +990,7 @@
         <v>12.8681551788903</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5216860731273602E-6</v>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
         <v>12.915730202065101</v>
       </c>
       <c r="C14">
-        <f>POWER(10, B14-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.9293947725883628E-6</v>
       </c>
       <c r="D14">
@@ -1012,7 +1012,7 @@
         <v>13.1148897257097</v>
       </c>
       <c r="F14">
-        <f>POWER(10, E14-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>6.215630465696085E-6</v>
       </c>
       <c r="G14">
@@ -1022,7 +1022,7 @@
         <v>12.964462600757299</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.396003826143235E-6</v>
       </c>
       <c r="J14">
@@ -1032,7 +1032,7 @@
         <v>12.955396540196601</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3051868114834216E-6</v>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
         <v>13.0041415683284</v>
       </c>
       <c r="C15">
-        <f>POWER(10, B15-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>4.8165606060603615E-6</v>
       </c>
       <c r="D15">
@@ -1054,7 +1054,7 @@
         <v>13.206864925030199</v>
       </c>
       <c r="F15">
-        <f>POWER(10, E15-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>7.6817538370536299E-6</v>
       </c>
       <c r="G15">
@@ -1064,7 +1064,7 @@
         <v>13.0478110982649</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.3260661887594399E-6</v>
       </c>
       <c r="J15">
@@ -1074,7 +1074,7 @@
         <v>13.0390160925283</v>
       </c>
       <c r="L15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2192915051122168E-6</v>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
         <v>13.0909428598091</v>
       </c>
       <c r="C16">
-        <f>POWER(10, B16-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>5.8821801438855626E-6</v>
       </c>
       <c r="D16">
@@ -1096,7 +1096,7 @@
         <v>13.299485149773499</v>
       </c>
       <c r="F16">
-        <f>POWER(10, E16-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>9.507812547766368E-6</v>
       </c>
       <c r="G16">
@@ -1106,7 +1106,7 @@
         <v>13.1322396128592</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.4689690579498688E-6</v>
       </c>
       <c r="J16">
@@ -1116,7 +1116,7 @@
         <v>13.119049040793501</v>
       </c>
       <c r="L16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.2754446264764857E-6</v>
       </c>
     </row>
@@ -1128,7 +1128,7 @@
         <v>13.179785664592799</v>
       </c>
       <c r="C17">
-        <f>POWER(10, B17-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>7.2174058217717719E-6</v>
       </c>
       <c r="D17">
@@ -1138,7 +1138,7 @@
         <v>13.3867086173784</v>
       </c>
       <c r="F17">
-        <f>POWER(10, E17-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.1622621057981298E-5</v>
       </c>
       <c r="G17">
@@ -1148,7 +1148,7 @@
         <v>13.216392911383601</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.8521461130833756E-6</v>
       </c>
       <c r="J17">
@@ -1158,7 +1158,7 @@
         <v>13.1972862360757</v>
       </c>
       <c r="L17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.5141817789278837E-6</v>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
         <v>13.2691914279293</v>
       </c>
       <c r="C18">
-        <f>POWER(10, B18-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>8.8672078570124654E-6</v>
       </c>
       <c r="D18">
@@ -1180,7 +1180,7 @@
         <v>13.469132668625999</v>
       </c>
       <c r="F18">
-        <f>POWER(10, E18-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.4051676072272072E-5</v>
       </c>
       <c r="G18">
@@ -1190,7 +1190,7 @@
         <v>13.301085476465801</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.5429124056088258E-6</v>
       </c>
       <c r="J18">
@@ -1200,7 +1200,7 @@
         <v>13.285638974969601</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.2094657261391616E-6</v>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
         <v>13.3580965535137</v>
       </c>
       <c r="C19">
-        <f>POWER(10, B19-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.0881581383602971E-5</v>
       </c>
       <c r="D19">
@@ -1222,7 +1222,7 @@
         <v>13.554965265239501</v>
       </c>
       <c r="F19">
-        <f>POWER(10, E19-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.7122245757253025E-5</v>
       </c>
       <c r="G19">
@@ -1232,7 +1232,7 @@
         <v>13.386320763804299</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1612245925461964E-5</v>
       </c>
       <c r="J19">
@@ -1242,7 +1242,7 @@
         <v>13.3697622487087</v>
       </c>
       <c r="L19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1177835389863527E-5</v>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
         <v>13.4475973537778</v>
       </c>
       <c r="C20">
-        <f>POWER(10, B20-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.3371890598295518E-5</v>
       </c>
       <c r="D20">
@@ -1264,7 +1264,7 @@
         <v>13.6408502245799</v>
       </c>
       <c r="F20">
-        <f>POWER(10, E20-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.0866311460010096E-5</v>
       </c>
       <c r="G20">
@@ -1274,7 +1274,7 @@
         <v>13.470985768511699</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4111761551172588E-5</v>
       </c>
       <c r="J20">
@@ -1284,7 +1284,7 @@
         <v>13.4544181822016</v>
       </c>
       <c r="L20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3583561181457722E-5</v>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
         <v>13.537697819811401</v>
       </c>
       <c r="C21">
-        <f>POWER(10, B21-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.6454825490517985E-5</v>
       </c>
       <c r="D21">
@@ -1306,7 +1306,7 @@
         <v>13.729020023658901</v>
       </c>
       <c r="F21">
-        <f>POWER(10, E21-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.5563215704251914E-5</v>
       </c>
       <c r="G21">
@@ -1316,7 +1316,7 @@
         <v>13.5539334823495</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7081615558449263E-5</v>
       </c>
       <c r="J21">
@@ -1326,7 +1326,7 @@
         <v>13.548645066438899</v>
       </c>
       <c r="L21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6874873559787811E-5</v>
       </c>
     </row>
@@ -1338,7 +1338,7 @@
         <v>13.627272533581101</v>
       </c>
       <c r="C22">
-        <f>POWER(10, B22-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.0224043678917554E-5</v>
       </c>
       <c r="D22">
@@ -1348,7 +1348,7 @@
         <v>13.830055250997599</v>
       </c>
       <c r="F22">
-        <f>POWER(10, E22-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.2258985995799319E-5</v>
       </c>
       <c r="G22">
@@ -1358,7 +1358,7 @@
         <v>13.6364119880323</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0654155815333156E-5</v>
       </c>
       <c r="J22">
@@ -1368,7 +1368,7 @@
         <v>13.631548087440301</v>
       </c>
       <c r="L22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.0424129169137591E-5</v>
       </c>
     </row>
@@ -1380,7 +1380,7 @@
         <v>13.7129516753619</v>
       </c>
       <c r="C23">
-        <f>POWER(10, B23-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.4634691974946078E-5</v>
       </c>
       <c r="D23">
@@ -1390,7 +1390,7 @@
         <v>13.9191268854527</v>
       </c>
       <c r="F23">
-        <f>POWER(10, E23-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.9602476637812306E-5</v>
       </c>
       <c r="G23">
@@ -1400,7 +1400,7 @@
         <v>13.7302609210961</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5636361211740782E-5</v>
       </c>
       <c r="J23">
@@ -1410,7 +1410,7 @@
         <v>13.718545357983899</v>
       </c>
       <c r="L23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.4954037246249327E-5</v>
       </c>
     </row>
@@ -1422,7 +1422,7 @@
         <v>13.7985361673336</v>
       </c>
       <c r="C24">
-        <f>POWER(10, B24-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.0000716591770054E-5</v>
       </c>
       <c r="D24">
@@ -1432,7 +1432,7 @@
         <v>14.0079594992993</v>
       </c>
       <c r="F24">
-        <f>POWER(10, E24-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>4.8590901919467273E-5</v>
       </c>
       <c r="G24">
@@ -1442,7 +1442,7 @@
         <v>13.8169428417792</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1299565071153124E-5</v>
       </c>
       <c r="J24">
@@ -1452,7 +1452,7 @@
         <v>13.804095628190201</v>
       </c>
       <c r="L24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.038722833150881E-5</v>
       </c>
     </row>
@@ -1464,7 +1464,7 @@
         <v>13.889221708320701</v>
       </c>
       <c r="C25">
-        <f>POWER(10, B25-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.6967252109001644E-5</v>
       </c>
       <c r="D25">
@@ -1474,7 +1474,7 @@
         <v>14.0944968844692</v>
       </c>
       <c r="F25">
-        <f>POWER(10, E25-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>5.9305141364087674E-5</v>
       </c>
       <c r="G25">
@@ -1484,7 +1484,7 @@
         <v>13.9041720030003</v>
       </c>
       <c r="I25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.826198208191486E-5</v>
       </c>
       <c r="J25">
@@ -1494,7 +1494,7 @@
         <v>13.888158870177501</v>
       </c>
       <c r="L25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.6876893678381349E-5</v>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
         <v>13.980052660725599</v>
       </c>
       <c r="C26">
-        <f>POWER(10, B26-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>4.5566757094917849E-5</v>
       </c>
       <c r="D26">
@@ -1516,7 +1516,7 @@
         <v>14.181974002371399</v>
       </c>
       <c r="F26">
-        <f>POWER(10, E26-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>7.2538649097431921E-5</v>
       </c>
       <c r="G26">
@@ -1526,7 +1526,7 @@
         <v>13.991951859599901</v>
       </c>
       <c r="I26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.6832497713620888E-5</v>
       </c>
       <c r="J26">
@@ -1536,7 +1536,7 @@
         <v>13.975983018544101</v>
       </c>
       <c r="L26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.5141759175100172E-5</v>
       </c>
     </row>
@@ -1548,7 +1548,7 @@
         <v>14.0753898023933</v>
       </c>
       <c r="C27">
-        <f>POWER(10, B27-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>5.6752534763427918E-5</v>
       </c>
       <c r="D27">
@@ -1558,7 +1558,7 @@
         <v>14.2655606790701</v>
       </c>
       <c r="F27">
-        <f>POWER(10, E27-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>8.7933860490093852E-5</v>
       </c>
       <c r="G27">
@@ -1568,7 +1568,7 @@
         <v>14.079947602579599</v>
       </c>
       <c r="I27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.7351273183520524E-5</v>
       </c>
       <c r="J27">
@@ -1578,7 +1578,7 @@
         <v>14.0639545790157</v>
       </c>
       <c r="L27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5277709601091373E-5</v>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
         <v>14.1693581360419</v>
       </c>
       <c r="C28">
-        <f>POWER(10, B28-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>7.0461777880322047E-5</v>
       </c>
       <c r="D28">
@@ -1600,7 +1600,7 @@
         <v>14.3373535873267</v>
       </c>
       <c r="F28">
-        <f>POWER(10, E28-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.0374066995172044E-4</v>
       </c>
       <c r="G28">
@@ -1610,7 +1610,7 @@
         <v>14.164464294762301</v>
       </c>
       <c r="I28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.9672237143221868E-5</v>
       </c>
       <c r="J28">
@@ -1620,7 +1620,7 @@
         <v>14.153151652153401</v>
       </c>
       <c r="L28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.7880825187836594E-5</v>
       </c>
     </row>
@@ -1632,7 +1632,7 @@
         <v>14.2699682918619</v>
       </c>
       <c r="C29">
-        <f>POWER(10, B29-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>8.8830836719025718E-5</v>
       </c>
       <c r="D29">
@@ -1642,7 +1642,7 @@
         <v>14.4068481960689</v>
       </c>
       <c r="F29">
-        <f>POWER(10, E29-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.2174290401552009E-4</v>
       </c>
       <c r="G29">
@@ -1652,7 +1652,7 @@
         <v>14.230118589989299</v>
       </c>
       <c r="I29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1042727903695246E-5</v>
       </c>
       <c r="J29">
@@ -1662,7 +1662,7 @@
         <v>14.2341347099907</v>
       </c>
       <c r="L29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.1795643040075301E-5</v>
       </c>
     </row>
@@ -1674,7 +1674,7 @@
         <v>14.3593674882838</v>
       </c>
       <c r="C30">
-        <f>POWER(10, B30-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.0913472269729516E-4</v>
       </c>
       <c r="D30">
@@ -1684,7 +1684,7 @@
         <v>14.4774431722184</v>
       </c>
       <c r="F30">
-        <f>POWER(10, E30-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.4323153070066073E-4</v>
       </c>
       <c r="G30">
@@ -1694,7 +1694,7 @@
         <v>14.295700219691501</v>
       </c>
       <c r="I30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.4253108149795441E-5</v>
       </c>
       <c r="J30">
@@ -1704,7 +1704,7 @@
         <v>14.3046377795037</v>
       </c>
       <c r="L30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.6212885681270382E-5</v>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
         <v>14.449745894741101</v>
       </c>
       <c r="C31">
-        <f>POWER(10, B31-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.3438207901154002E-4</v>
       </c>
       <c r="D31">
@@ -1726,7 +1726,7 @@
         <v>14.547937563950001</v>
       </c>
       <c r="F31">
-        <f>POWER(10, E31-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.6847405341825276E-4</v>
       </c>
       <c r="G31">
@@ -1736,7 +1736,7 @@
         <v>14.361962811990701</v>
       </c>
       <c r="I31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0978885934334265E-4</v>
       </c>
       <c r="J31">
@@ -1746,7 +1746,7 @@
         <v>14.3751109810988</v>
       </c>
       <c r="L31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1316351848283813E-4</v>
       </c>
     </row>
@@ -1758,7 +1758,7 @@
         <v>14.543537265678101</v>
       </c>
       <c r="C32">
-        <f>POWER(10, B32-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.6677568252572821E-4</v>
       </c>
       <c r="D32">
@@ -1768,7 +1768,7 @@
         <v>14.6588509468884</v>
       </c>
       <c r="F32">
-        <f>POWER(10, E32-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.1749356294912167E-4</v>
       </c>
       <c r="G32">
@@ -1778,7 +1778,7 @@
         <v>14.4285325407764</v>
       </c>
       <c r="I32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.279758438130177E-4</v>
       </c>
       <c r="J32">
@@ -1788,7 +1788,7 @@
         <v>14.4463123199512</v>
       </c>
       <c r="L32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3332382993118492E-4</v>
       </c>
     </row>
@@ -1800,7 +1800,7 @@
         <v>14.6144166446126</v>
       </c>
       <c r="C33">
-        <f>POWER(10, B33-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.963415004659225E-4</v>
       </c>
       <c r="D33">
@@ -1810,7 +1810,7 @@
         <v>14.783185633839301</v>
       </c>
       <c r="F33">
-        <f>POWER(10, E33-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.8958835560872917E-4</v>
       </c>
       <c r="G33">
@@ -1820,7 +1820,7 @@
         <v>14.495410829669799</v>
       </c>
       <c r="I33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4928160325353274E-4</v>
       </c>
       <c r="J33">
@@ -1830,7 +1830,7 @@
         <v>14.517866326039499</v>
       </c>
       <c r="L33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5720334653301351E-4</v>
       </c>
     </row>
@@ -1842,7 +1842,7 @@
         <v>14.6771242067115</v>
       </c>
       <c r="C34">
-        <f>POWER(10, B34-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.2684001519324647E-4</v>
       </c>
       <c r="D34">
@@ -1852,7 +1852,7 @@
         <v>14.9180955979009</v>
       </c>
       <c r="F34">
-        <f>POWER(10, E34-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.9508547081907003E-4</v>
       </c>
       <c r="G34">
@@ -1862,7 +1862,7 @@
         <v>14.562215098334301</v>
       </c>
       <c r="I34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7410472572152997E-4</v>
       </c>
       <c r="J34">
@@ -1872,7 +1872,7 @@
         <v>14.5897747461592</v>
       </c>
       <c r="L34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8551123094169336E-4</v>
       </c>
     </row>
@@ -1884,7 +1884,7 @@
         <v>14.7393234623399</v>
       </c>
       <c r="C35">
-        <f>POWER(10, B35-10)/$N$3</f>
+        <f t="shared" ref="C35:C66" si="4">POWER(10, B35-10)/$N$3</f>
         <v>2.6176942759085267E-4</v>
       </c>
       <c r="D35">
@@ -1894,7 +1894,7 @@
         <v>15.0572400734886</v>
       </c>
       <c r="F35">
-        <f>POWER(10, E35-10)/$N$3</f>
+        <f t="shared" ref="F35:F66" si="5">POWER(10, E35-10)/$N$3</f>
         <v>5.4429649098266001E-4</v>
       </c>
       <c r="G35">
@@ -1904,7 +1904,7 @@
         <v>14.629713024788</v>
       </c>
       <c r="I35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0338011369399996E-4</v>
       </c>
       <c r="J35">
@@ -1914,7 +1914,7 @@
         <v>14.661266080433901</v>
       </c>
       <c r="L35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.1870642490360497E-4</v>
       </c>
     </row>
@@ -1926,7 +1926,7 @@
         <v>14.802566974810301</v>
       </c>
       <c r="C36">
-        <f>POWER(10, B36-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.0280457728310413E-4</v>
       </c>
       <c r="D36">
@@ -1936,7 +1936,7 @@
         <v>15.1954783459481</v>
       </c>
       <c r="F36">
-        <f>POWER(10, E36-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>7.4829666029612016E-4</v>
       </c>
       <c r="G36">
@@ -1946,7 +1946,7 @@
         <v>14.6975238136769</v>
       </c>
       <c r="I36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3774931518579195E-4</v>
       </c>
       <c r="J36">
@@ -1956,7 +1956,7 @@
         <v>14.733496246346</v>
       </c>
       <c r="L36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5828055284620377E-4</v>
       </c>
     </row>
@@ -1968,7 +1968,7 @@
         <v>14.868117870608501</v>
       </c>
       <c r="C37">
-        <f>POWER(10, B37-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.5213835539414602E-4</v>
       </c>
       <c r="D37">
@@ -1978,7 +1978,7 @@
         <v>15.3349857633425</v>
       </c>
       <c r="F37">
-        <f>POWER(10, E37-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.0317660284054682E-3</v>
       </c>
       <c r="G37">
@@ -1988,7 +1988,7 @@
         <v>14.7656489151624</v>
       </c>
       <c r="I37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7812778439112364E-4</v>
       </c>
       <c r="J37">
@@ -1998,7 +1998,7 @@
         <v>14.7877431236732</v>
       </c>
       <c r="L37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.9264329944102421E-4</v>
       </c>
     </row>
@@ -2010,7 +2010,7 @@
         <v>15.0081114038768</v>
       </c>
       <c r="C38">
-        <f>POWER(10, B38-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>4.8607900688169556E-4</v>
       </c>
       <c r="D38">
@@ -2020,7 +2020,7 @@
         <v>15.483638635761899</v>
       </c>
       <c r="F38">
-        <f>POWER(10, E38-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.4528945569562887E-3</v>
       </c>
       <c r="G38">
@@ -2030,7 +2030,7 @@
         <v>14.834480966111901</v>
       </c>
       <c r="I38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2589404675998913E-4</v>
       </c>
       <c r="J38">
@@ -2040,7 +2040,7 @@
         <v>14.831234900160901</v>
       </c>
       <c r="L38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2346728337892549E-4</v>
       </c>
     </row>
@@ -2052,7 +2052,7 @@
         <v>15.157055652880301</v>
       </c>
       <c r="C39">
-        <f>POWER(10, B39-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>6.8493776747319962E-4</v>
       </c>
       <c r="D39">
@@ -2062,7 +2062,7 @@
         <v>15.6280580600794</v>
       </c>
       <c r="F39">
-        <f>POWER(10, E39-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.0260656850044872E-3</v>
       </c>
       <c r="G39">
@@ -2072,7 +2072,7 @@
         <v>14.9032408833683</v>
       </c>
       <c r="I39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8180036949831092E-4</v>
       </c>
       <c r="J39">
@@ -2082,7 +2082,7 @@
         <v>14.8752468439405</v>
       </c>
       <c r="L39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5796643362891612E-4</v>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
         <v>15.300478548628501</v>
       </c>
       <c r="C40">
-        <f>POWER(10, B40-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>9.5295854713663066E-4</v>
       </c>
       <c r="D40">
@@ -2104,7 +2104,7 @@
         <v>15.770774470942101</v>
       </c>
       <c r="F40">
-        <f>POWER(10, E40-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.8142970272283341E-3</v>
       </c>
       <c r="G40">
@@ -2114,7 +2114,7 @@
         <v>14.971924697828101</v>
       </c>
       <c r="I40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.4721891004391852E-4</v>
       </c>
       <c r="J40">
@@ -2124,7 +2124,7 @@
         <v>14.918995974928601</v>
       </c>
       <c r="L40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9590540958461058E-4</v>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
         <v>15.439455190953799</v>
       </c>
       <c r="C41">
-        <f>POWER(10, B41-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.3123529503590943E-3</v>
       </c>
       <c r="D41">
@@ -2146,7 +2146,7 @@
         <v>15.901584187607201</v>
       </c>
       <c r="F41">
-        <f>POWER(10, E41-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.8034669654698557E-3</v>
       </c>
       <c r="G41">
@@ -2156,7 +2156,7 @@
         <v>15.041321686219</v>
       </c>
       <c r="I41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.2470734934121916E-4</v>
       </c>
       <c r="J41">
@@ -2166,7 +2166,7 @@
         <v>14.963268351201799</v>
       </c>
       <c r="L41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3839320311694354E-4</v>
       </c>
     </row>
@@ -2178,7 +2178,7 @@
         <v>15.592448258200999</v>
       </c>
       <c r="C42">
-        <f>POWER(10, B42-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.8665675834324362E-3</v>
       </c>
       <c r="D42">
@@ -2188,7 +2188,7 @@
         <v>16.422895846885002</v>
       </c>
       <c r="F42">
-        <f>POWER(10, E42-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.2632558203024141E-2</v>
       </c>
       <c r="G42">
@@ -2198,7 +2198,7 @@
         <v>15.1038694372879</v>
       </c>
       <c r="I42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0598921965031066E-4</v>
       </c>
       <c r="J42">
@@ -2208,7 +2208,7 @@
         <v>15.007672106510499</v>
       </c>
       <c r="L42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.8558757704246042E-4</v>
       </c>
     </row>
@@ -2220,7 +2220,7 @@
         <v>15.745553223326899</v>
       </c>
       <c r="C43">
-        <f>POWER(10, B43-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.6555145437939898E-3</v>
       </c>
       <c r="D43">
@@ -2230,7 +2230,7 @@
         <v>16.318440571332498</v>
       </c>
       <c r="F43">
-        <f>POWER(10, E43-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>9.9319844818487896E-3</v>
       </c>
       <c r="G43">
@@ -2240,7 +2240,7 @@
         <v>15.147092629628199</v>
       </c>
       <c r="I43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.6940367242704899E-4</v>
       </c>
       <c r="J43">
@@ -2250,7 +2250,7 @@
         <v>15.0526045625497</v>
       </c>
       <c r="L43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.3851775118703919E-4</v>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
         <v>15.8924225799748</v>
       </c>
       <c r="C44">
-        <f>POWER(10, B44-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.7240717604682836E-3</v>
       </c>
       <c r="D44">
@@ -2272,7 +2272,7 @@
         <v>16.214649667319001</v>
       </c>
       <c r="F44">
-        <f>POWER(10, E44-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>7.8206910235430419E-3</v>
       </c>
       <c r="G44">
@@ -2282,7 +2282,7 @@
         <v>15.1892378472988</v>
       </c>
       <c r="I44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.3762106071058222E-4</v>
       </c>
       <c r="J44">
@@ -2292,7 +2292,7 @@
         <v>15.0972734245968</v>
       </c>
       <c r="L44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.968550675874121E-4</v>
       </c>
     </row>
@@ -2304,7 +2304,7 @@
         <v>16.028037371805599</v>
       </c>
       <c r="C45">
-        <f>POWER(10, B45-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>5.0890044753188418E-3</v>
       </c>
       <c r="D45">
@@ -2314,7 +2314,7 @@
         <v>16.116193053934399</v>
       </c>
       <c r="F45">
-        <f>POWER(10, E45-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>6.2343117402355232E-3</v>
       </c>
       <c r="G45">
@@ -2324,7 +2324,7 @@
         <v>15.2315003296759</v>
       </c>
       <c r="I45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1300981884360973E-4</v>
       </c>
       <c r="J45">
@@ -2334,7 +2334,7 @@
         <v>15.1420748422576</v>
       </c>
       <c r="L45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.6171396962183245E-4</v>
       </c>
     </row>
@@ -2346,7 +2346,7 @@
         <v>16.193293613335701</v>
       </c>
       <c r="C46">
-        <f>POWER(10, B46-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>7.4454178188106367E-3</v>
       </c>
       <c r="D46">
@@ -2356,7 +2356,7 @@
         <v>16.013688513809299</v>
       </c>
       <c r="F46">
-        <f>POWER(10, E46-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>4.9236137380389289E-3</v>
       </c>
       <c r="G46">
@@ -2366,7 +2366,7 @@
         <v>15.2730748800759</v>
       </c>
       <c r="I46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.9468538091711988E-4</v>
       </c>
       <c r="J46">
@@ -2376,7 +2376,7 @@
         <v>15.187009208893301</v>
       </c>
       <c r="L46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.3384555818926196E-4</v>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
         <v>16.350592407533501</v>
       </c>
       <c r="C47">
-        <f>POWER(10, B47-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.0695174345101881E-2</v>
       </c>
       <c r="D47">
@@ -2398,7 +2398,7 @@
         <v>15.819806217283199</v>
       </c>
       <c r="F47">
-        <f>POWER(10, E47-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.1506610082628365E-3</v>
       </c>
       <c r="G47">
@@ -2408,7 +2408,7 @@
         <v>15.315570630320501</v>
       </c>
       <c r="I47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.8665674987890618E-4</v>
       </c>
       <c r="J47">
@@ -2418,7 +2418,7 @@
         <v>15.232076919032099</v>
       </c>
       <c r="L47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.1408992496404616E-4</v>
       </c>
     </row>
@@ -2430,7 +2430,7 @@
         <v>16.489680931441001</v>
       </c>
       <c r="C48">
-        <f>POWER(10, B48-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.4732498055012927E-2</v>
       </c>
       <c r="D48">
@@ -2440,7 +2440,7 @@
         <v>15.719186799549499</v>
       </c>
       <c r="F48">
-        <f>POWER(10, E48-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.4990920936558162E-3</v>
       </c>
       <c r="G48">
@@ -2450,7 +2450,7 @@
         <v>15.357779630729301</v>
       </c>
       <c r="I48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0873643536775141E-3</v>
       </c>
       <c r="J48">
@@ -2460,7 +2460,7 @@
         <v>15.277278368373301</v>
       </c>
       <c r="L48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.0338698484964265E-4</v>
       </c>
     </row>
@@ -2472,7 +2472,7 @@
         <v>16.6241547750191</v>
       </c>
       <c r="C49">
-        <f>POWER(10, B49-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.0079377098077767E-2</v>
       </c>
       <c r="D49">
@@ -2482,7 +2482,7 @@
         <v>15.0388735727584</v>
       </c>
       <c r="F49">
-        <f>POWER(10, E49-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>5.2175790030750777E-4</v>
       </c>
       <c r="G49">
@@ -2492,7 +2492,7 @@
         <v>15.4005110631765</v>
       </c>
       <c r="I49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.199793553574433E-3</v>
       </c>
       <c r="J49">
@@ -2502,7 +2502,7 @@
         <v>15.322613953790199</v>
       </c>
       <c r="L49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0027886615483082E-3</v>
       </c>
     </row>
@@ -2514,7 +2514,7 @@
         <v>15.886091580888699</v>
       </c>
       <c r="C50">
-        <f>POWER(10, B50-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.6701772754531552E-3</v>
       </c>
       <c r="D50">
@@ -2524,7 +2524,7 @@
         <v>15.6237386752176</v>
       </c>
       <c r="F50">
-        <f>POWER(10, E50-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.006014815561051E-3</v>
       </c>
       <c r="G50">
@@ -2534,7 +2534,7 @@
         <v>15.442954155468099</v>
       </c>
       <c r="I50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3229688434311286E-3</v>
       </c>
       <c r="J50">
@@ -2544,7 +2544,7 @@
         <v>15.3676788224258</v>
       </c>
       <c r="L50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1124340753426673E-3</v>
       </c>
     </row>
@@ -2556,7 +2556,7 @@
         <v>15.7476481575384</v>
       </c>
       <c r="C51">
-        <f>POWER(10, B51-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.6683550649369797E-3</v>
       </c>
       <c r="D51">
@@ -2566,7 +2566,7 @@
         <v>15.524366314600099</v>
       </c>
       <c r="F51">
-        <f>POWER(10, E51-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.5957386921863226E-3</v>
       </c>
       <c r="G51">
@@ -2576,7 +2576,7 @@
         <v>15.4859225772156</v>
       </c>
       <c r="I51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4605554116272899E-3</v>
       </c>
       <c r="J51">
@@ -2586,7 +2586,7 @@
         <v>15.412876229960601</v>
       </c>
       <c r="L51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.2344448465027751E-3</v>
       </c>
     </row>
@@ -2598,7 +2598,7 @@
         <v>16.046201856716301</v>
       </c>
       <c r="C52">
-        <f>POWER(10, B52-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>5.3063674186165193E-3</v>
       </c>
       <c r="D52">
@@ -2608,7 +2608,7 @@
         <v>14.911994971840301</v>
       </c>
       <c r="F52">
-        <f>POWER(10, E52-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.8957442006258319E-4</v>
       </c>
       <c r="G52">
@@ -2618,7 +2618,7 @@
         <v>15.528601059667899</v>
       </c>
       <c r="I52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.611374626172732E-3</v>
       </c>
       <c r="J52">
@@ -2628,7 +2628,7 @@
         <v>15.4586142043559</v>
       </c>
       <c r="L52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3715437496906581E-3</v>
       </c>
     </row>
@@ -2640,7 +2640,7 @@
         <v>15.6491898570051</v>
       </c>
       <c r="C53">
-        <f>POWER(10, B53-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.1270873166332254E-3</v>
       </c>
       <c r="D53">
@@ -2650,7 +2650,7 @@
         <v>15.4301011553991</v>
       </c>
       <c r="F53">
-        <f>POWER(10, E53-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.2843891151728931E-3</v>
       </c>
       <c r="G53">
@@ -2660,7 +2660,7 @@
         <v>15.5718077850628</v>
       </c>
       <c r="I53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.779931324111343E-3</v>
       </c>
       <c r="J53">
@@ -2670,7 +2670,7 @@
         <v>15.5044879069742</v>
       </c>
       <c r="L53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5243453418392751E-3</v>
       </c>
     </row>
@@ -2682,7 +2682,7 @@
         <v>15.5513471428023</v>
       </c>
       <c r="C54">
-        <f>POWER(10, B54-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.6980192280036249E-3</v>
       </c>
       <c r="D54">
@@ -2692,7 +2692,7 @@
         <v>14.7801052199758</v>
       </c>
       <c r="F54">
-        <f>POWER(10, E54-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.875415973273757E-4</v>
       </c>
       <c r="G54">
@@ -2702,7 +2702,7 @@
         <v>15.614722963153801</v>
       </c>
       <c r="I54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9648003378760904E-3</v>
       </c>
       <c r="J54">
@@ -2712,7 +2712,7 @@
         <v>15.5509078124963</v>
       </c>
       <c r="L54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6963023880606641E-3</v>
       </c>
     </row>
@@ -2724,7 +2724,7 @@
         <v>16.148935841278501</v>
       </c>
       <c r="C55">
-        <f>POWER(10, B55-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>6.7225076060410749E-3</v>
       </c>
       <c r="D55">
@@ -2734,7 +2734,7 @@
         <v>15.336408381573399</v>
       </c>
       <c r="F55">
-        <f>POWER(10, E55-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.0351513254822707E-3</v>
       </c>
       <c r="G55">
@@ -2744,7 +2744,7 @@
         <v>15.658169313832399</v>
       </c>
       <c r="I55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.1715247060779723E-3</v>
       </c>
       <c r="J55">
@@ -2754,7 +2754,7 @@
         <v>15.5970553979787</v>
       </c>
       <c r="L55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8864741519414967E-3</v>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
         <v>15.454676523047301</v>
       </c>
       <c r="C56">
-        <f>POWER(10, B56-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.3591643790747197E-3</v>
       </c>
       <c r="D56">
@@ -2776,7 +2776,7 @@
         <v>14.702644813377001</v>
       </c>
       <c r="F56">
-        <f>POWER(10, E56-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.4056933870013713E-4</v>
       </c>
       <c r="G56">
@@ -2786,7 +2786,7 @@
         <v>15.7009084619937</v>
       </c>
       <c r="I56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3960943935805975E-3</v>
       </c>
       <c r="J56">
@@ -2796,7 +2796,7 @@
         <v>15.643339927212001</v>
       </c>
       <c r="L56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.0986276388295783E-3</v>
       </c>
     </row>
@@ -2808,7 +2808,7 @@
         <v>15.3586068292853</v>
       </c>
       <c r="C57">
-        <f>POWER(10, B57-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.0894374248522046E-3</v>
       </c>
       <c r="D57">
@@ -2818,7 +2818,7 @@
         <v>15.2388635406136</v>
       </c>
       <c r="F57">
-        <f>POWER(10, E57-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>8.2691144254515303E-4</v>
       </c>
       <c r="G57">
@@ -2828,7 +2828,7 @@
         <v>15.7450098052089</v>
       </c>
       <c r="I57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.6521938654771753E-3</v>
       </c>
       <c r="J57">
@@ -2838,7 +2838,7 @@
         <v>15.689348073143799</v>
       </c>
       <c r="L57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.3331546917117162E-3</v>
       </c>
     </row>
@@ -2850,7 +2850,7 @@
         <v>15.2625809140601</v>
       </c>
       <c r="C58">
-        <f>POWER(10, B58-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>8.7332597026559627E-4</v>
       </c>
       <c r="D58">
@@ -2860,7 +2860,7 @@
         <v>14.7112246582181</v>
       </c>
       <c r="F58">
-        <f>POWER(10, E58-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.4536924082936459E-4</v>
       </c>
       <c r="G58">
@@ -2870,7 +2870,7 @@
         <v>15.7879859854621</v>
       </c>
       <c r="I58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.9280699424703324E-3</v>
       </c>
       <c r="J58">
@@ -2880,7 +2880,7 @@
         <v>15.7359064824726</v>
       </c>
       <c r="L58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5971793637258305E-3</v>
       </c>
     </row>
@@ -2892,7 +2892,7 @@
         <v>15.171475566623799</v>
       </c>
       <c r="C59">
-        <f>POWER(10, B59-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>7.080615763510003E-4</v>
       </c>
       <c r="D59">
@@ -2902,7 +2902,7 @@
         <v>14.765681510414201</v>
       </c>
       <c r="F59">
-        <f>POWER(10, E59-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.7814865959390595E-4</v>
       </c>
       <c r="G59">
@@ -2912,7 +2912,7 @@
         <v>15.8323319155277</v>
       </c>
       <c r="I59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2428538524660608E-3</v>
       </c>
       <c r="J59">
@@ -2922,7 +2922,7 @@
         <v>15.784684127437901</v>
       </c>
       <c r="L59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.9058927968932369E-3</v>
       </c>
     </row>
@@ -2934,7 +2934,7 @@
         <v>15.2036623114639</v>
       </c>
       <c r="C60">
-        <f>POWER(10, B60-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>7.6253147095987699E-4</v>
       </c>
       <c r="D60">
@@ -2944,7 +2944,7 @@
         <v>14.753614960837099</v>
       </c>
       <c r="F60">
-        <f>POWER(10, E60-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.7052687876677744E-4</v>
       </c>
       <c r="G60">
@@ -2954,7 +2954,7 @@
         <v>15.8734533902955</v>
       </c>
       <c r="I60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.5649123081728856E-3</v>
       </c>
       <c r="J60">
@@ -2964,7 +2964,7 @@
         <v>15.8357007705992</v>
       </c>
       <c r="L60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2681067321516954E-3</v>
       </c>
     </row>
@@ -2976,7 +2976,7 @@
         <v>15.245160877682</v>
       </c>
       <c r="C61">
-        <f>POWER(10, B61-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>8.3898913880173025E-4</v>
       </c>
       <c r="D61">
@@ -2986,7 +2986,7 @@
         <v>14.7871324668579</v>
       </c>
       <c r="F61">
-        <f>POWER(10, E61-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.9223210598995999E-4</v>
       </c>
       <c r="G61">
@@ -2996,7 +2996,7 @@
         <v>15.909226894981099</v>
       </c>
       <c r="I61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8709927325660874E-3</v>
       </c>
       <c r="J61">
@@ -3006,7 +3006,7 @@
         <v>15.885625540152599</v>
       </c>
       <c r="L61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.6662409263243227E-3</v>
       </c>
     </row>
@@ -3018,7 +3018,7 @@
         <v>15.287982098751201</v>
       </c>
       <c r="C62">
-        <f>POWER(10, B62-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>9.2592873002832633E-4</v>
       </c>
       <c r="D62">
@@ -3028,7 +3028,7 @@
         <v>14.8224119696843</v>
       </c>
       <c r="F62">
-        <f>POWER(10, E62-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.1696216940496586E-4</v>
       </c>
       <c r="G62">
@@ -3038,7 +3038,7 @@
         <v>15.943819656219301</v>
       </c>
       <c r="I62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.1919405726288574E-3</v>
       </c>
       <c r="J62">
@@ -3048,7 +3048,7 @@
         <v>15.9348672793249</v>
       </c>
       <c r="L62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.1064140796118727E-3</v>
       </c>
     </row>
@@ -3060,7 +3060,7 @@
         <v>15.33011506645</v>
       </c>
       <c r="C63">
-        <f>POWER(10, B63-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.0202592183400938E-3</v>
       </c>
       <c r="D63">
@@ -3070,7 +3070,7 @@
         <v>14.862477980242801</v>
       </c>
       <c r="F63">
-        <f>POWER(10, E63-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.4759493640716975E-4</v>
       </c>
       <c r="G63">
@@ -3080,7 +3080,7 @@
         <v>15.9780662883558</v>
       </c>
       <c r="I63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.5358820145446413E-3</v>
       </c>
       <c r="J63">
@@ -3090,7 +3090,7 @@
         <v>15.985947764739601</v>
       </c>
       <c r="L63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6189496243889154E-3</v>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
         <v>15.3723641506484</v>
       </c>
       <c r="C64">
-        <f>POWER(10, B64-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.1245003932235326E-3</v>
       </c>
       <c r="D64">
@@ -3112,7 +3112,7 @@
         <v>14.9038312871063</v>
       </c>
       <c r="F64">
-        <f>POWER(10, E64-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.8231976282671466E-4</v>
       </c>
       <c r="G64">
@@ -3122,7 +3122,7 @@
         <v>16.015342479089501</v>
       </c>
       <c r="I64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.9424005590306807E-3</v>
       </c>
       <c r="J64">
@@ -3132,7 +3132,7 @@
         <v>16.035500479441598</v>
       </c>
       <c r="L64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1772118962899053E-3</v>
       </c>
     </row>
@@ -3144,7 +3144,7 @@
         <v>15.4139167202051</v>
       </c>
       <c r="C65">
-        <f>POWER(10, B65-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.237405896505595E-3</v>
       </c>
       <c r="D65">
@@ -3154,7 +3154,7 @@
         <v>14.944905553032999</v>
       </c>
       <c r="F65">
-        <f>POWER(10, E65-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>4.2024350889244608E-4</v>
       </c>
       <c r="G65">
@@ -3164,7 +3164,7 @@
         <v>16.056939289032901</v>
       </c>
       <c r="I65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.439196516481757E-3</v>
       </c>
       <c r="J65">
@@ -3174,7 +3174,7 @@
         <v>16.086479346667399</v>
       </c>
       <c r="L65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.8220349426721194E-3</v>
       </c>
     </row>
@@ -3186,7 +3186,7 @@
         <v>15.4572119494725</v>
       </c>
       <c r="C66">
-        <f>POWER(10, B66-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.3671224355180185E-3</v>
       </c>
       <c r="D66">
@@ -3196,7 +3196,7 @@
         <v>14.9837221063926</v>
       </c>
       <c r="F66">
-        <f>POWER(10, E66-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>4.5953391312193178E-4</v>
       </c>
       <c r="G66">
@@ -3206,7 +3206,7 @@
         <v>16.1007668842987</v>
       </c>
       <c r="I66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0167552458473914E-3</v>
       </c>
       <c r="J66">
@@ -3216,7 +3216,7 @@
         <v>16.137620282105999</v>
       </c>
       <c r="L66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.549614563975791E-3</v>
       </c>
     </row>
@@ -3228,7 +3228,7 @@
         <v>15.499402582261601</v>
       </c>
       <c r="C67">
-        <f>POWER(10, B67-10)/$N$3</f>
+        <f t="shared" ref="C67:C98" si="6">POWER(10, B67-10)/$N$3</f>
         <v>1.5066002780657472E-3</v>
       </c>
       <c r="D67">
@@ -3238,7 +3238,7 @@
         <v>15.022243336719299</v>
       </c>
       <c r="F67">
-        <f>POWER(10, E67-10)/$N$3</f>
+        <f t="shared" ref="F67:F98" si="7">POWER(10, E67-10)/$N$3</f>
         <v>5.0215616360133281E-4</v>
       </c>
       <c r="G67">
@@ -3248,7 +3248,7 @@
         <v>16.144288377110101</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I116" si="2">POWER(10, H67-10)/$N$3</f>
+        <f t="shared" ref="I67:I116" si="8">POWER(10, H67-10)/$N$3</f>
         <v>6.6509523761772221E-3</v>
       </c>
       <c r="J67">
@@ -3258,7 +3258,7 @@
         <v>16.187643146284898</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L115" si="3">POWER(10, K67-10)/$N$3</f>
+        <f t="shared" ref="L67:L115" si="9">POWER(10, K67-10)/$N$3</f>
         <v>7.3491753091174897E-3</v>
       </c>
     </row>
@@ -3270,7 +3270,7 @@
         <v>15.5429379276568</v>
       </c>
       <c r="C68">
-        <f>POWER(10, B68-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.6654568635227928E-3</v>
       </c>
       <c r="D68">
@@ -3280,7 +3280,7 @@
         <v>15.0604664505816</v>
       </c>
       <c r="F68">
-        <f>POWER(10, E68-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>5.4835513102685759E-4</v>
       </c>
       <c r="G68">
@@ -3290,7 +3290,7 @@
         <v>16.183533039270401</v>
       </c>
       <c r="I68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.279951739129634E-3</v>
       </c>
       <c r="J68">
@@ -3300,7 +3300,7 @@
         <v>16.2391056941307</v>
       </c>
       <c r="L68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.2737263963041912E-3</v>
       </c>
     </row>
@@ -3312,7 +3312,7 @@
         <v>15.5853625504615</v>
       </c>
       <c r="C69">
-        <f>POWER(10, B69-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.8363607913557145E-3</v>
       </c>
       <c r="D69">
@@ -3322,7 +3322,7 @@
         <v>15.0983886710174</v>
       </c>
       <c r="F69">
-        <f>POWER(10, E69-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>5.9838973105477223E-4</v>
       </c>
       <c r="G69">
@@ -3332,7 +3332,7 @@
         <v>16.185472159524899</v>
       </c>
       <c r="I69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.3125293215731395E-3</v>
       </c>
       <c r="J69">
@@ -3342,7 +3342,7 @@
         <v>16.290302267068999</v>
       </c>
       <c r="L69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.3088863483356925E-3</v>
       </c>
     </row>
@@ -3354,7 +3354,7 @@
         <v>15.629551489383701</v>
       </c>
       <c r="C70">
-        <f>POWER(10, B70-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.0330448072793422E-3</v>
       </c>
       <c r="D70">
@@ -3364,7 +3364,7 @@
         <v>15.1332135410116</v>
       </c>
       <c r="F70">
-        <f>POWER(10, E70-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>6.4834923388527865E-4</v>
       </c>
       <c r="G70">
@@ -3374,7 +3374,7 @@
         <v>16.225108964281901</v>
       </c>
       <c r="I70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.0113263817750829E-3</v>
       </c>
       <c r="J70">
@@ -3384,7 +3384,7 @@
         <v>16.340367508800501</v>
       </c>
       <c r="L70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.0446311447324682E-2</v>
       </c>
     </row>
@@ -3396,7 +3396,7 @@
         <v>15.672625806438401</v>
       </c>
       <c r="C71">
-        <f>POWER(10, B71-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.2450254439194055E-3</v>
       </c>
       <c r="D71">
@@ -3406,7 +3406,7 @@
         <v>15.169318732541401</v>
       </c>
       <c r="F71">
-        <f>POWER(10, E71-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>7.0455385179363738E-4</v>
       </c>
       <c r="G71">
@@ -3416,7 +3416,7 @@
         <v>16.268108559979801</v>
       </c>
       <c r="I71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.8451259408900296E-3</v>
       </c>
       <c r="J71">
@@ -3426,7 +3426,7 @@
         <v>16.381512517204001</v>
       </c>
       <c r="L71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1484391212522852E-2</v>
       </c>
     </row>
@@ -3438,7 +3438,7 @@
         <v>15.7162332657861</v>
       </c>
       <c r="C72">
-        <f>POWER(10, B72-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.4821540222590638E-3</v>
       </c>
       <c r="D72">
@@ -3448,7 +3448,7 @@
         <v>15.2051091008322</v>
       </c>
       <c r="F72">
-        <f>POWER(10, E72-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>7.6507597043345467E-4</v>
       </c>
       <c r="G72">
@@ -3458,7 +3458,7 @@
         <v>16.308641556098902</v>
       </c>
       <c r="I72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.7103976957479306E-3</v>
       </c>
       <c r="J72">
@@ -3468,7 +3468,7 @@
         <v>16.417565133879801</v>
       </c>
       <c r="L72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.2478448611971298E-2</v>
       </c>
     </row>
@@ -3480,7 +3480,7 @@
         <v>15.759130900153201</v>
       </c>
       <c r="C73">
-        <f>POWER(10, B73-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.7398473138639939E-3</v>
       </c>
       <c r="D73">
@@ -3490,7 +3490,7 @@
         <v>15.240582013307399</v>
       </c>
       <c r="F73">
-        <f>POWER(10, E73-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>8.3018995505880499E-4</v>
       </c>
       <c r="G73">
@@ -3500,7 +3500,7 @@
         <v>16.345395830721898</v>
       </c>
       <c r="I73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.0567963185725783E-2</v>
       </c>
       <c r="J73">
@@ -3510,7 +3510,7 @@
         <v>16.454564886158099</v>
       </c>
       <c r="L73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.3588150461003069E-2</v>
       </c>
     </row>
@@ -3522,7 +3522,7 @@
         <v>15.803812521806799</v>
       </c>
       <c r="C74">
-        <f>POWER(10, B74-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.0367426065317652E-3</v>
       </c>
       <c r="D74">
@@ -3532,7 +3532,7 @@
         <v>15.2761376826711</v>
       </c>
       <c r="F74">
-        <f>POWER(10, E74-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>9.010173288855806E-4</v>
       </c>
       <c r="G74">
@@ -3542,7 +3542,7 @@
         <v>16.380936990518698</v>
       </c>
       <c r="I74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.1469182186583734E-2</v>
       </c>
       <c r="J74">
@@ -3552,7 +3552,7 @@
         <v>16.490778277307701</v>
       </c>
       <c r="L74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.4769770201280319E-2</v>
       </c>
     </row>
@@ -3564,7 +3564,7 @@
         <v>15.8473670941629</v>
       </c>
       <c r="C75">
-        <f>POWER(10, B75-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.3570866821204365E-3</v>
       </c>
       <c r="D75">
@@ -3574,7 +3574,7 @@
         <v>15.3117763019919</v>
       </c>
       <c r="F75">
-        <f>POWER(10, E75-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>9.7807410970044231E-4</v>
       </c>
       <c r="G75">
@@ -3584,7 +3584,7 @@
         <v>16.4169883405688</v>
       </c>
       <c r="I75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.2461886789154731E-2</v>
       </c>
       <c r="J75">
@@ -3594,7 +3594,7 @@
         <v>16.527943027753999</v>
       </c>
       <c r="L75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.6089349611942163E-2</v>
       </c>
     </row>
@@ -3606,7 +3606,7 @@
         <v>15.8914607530597</v>
       </c>
       <c r="C76">
-        <f>POWER(10, B76-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.7158332285072639E-3</v>
       </c>
       <c r="D76">
@@ -3616,7 +3616,7 @@
         <v>15.3462839726176</v>
       </c>
       <c r="F76">
-        <f>POWER(10, E76-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.0589597019291606E-3</v>
       </c>
       <c r="G76">
@@ -3626,7 +3626,7 @@
         <v>16.452685169941201</v>
       </c>
       <c r="I76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.3529465231820763E-2</v>
       </c>
       <c r="J76">
@@ -3636,7 +3636,7 @@
         <v>16.564317910341501</v>
       </c>
       <c r="L76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.7494976817259793E-2</v>
       </c>
     </row>
@@ -3648,7 +3648,7 @@
         <v>15.935256879865101</v>
       </c>
       <c r="C77">
-        <f>POWER(10, B77-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>4.1100995488809319E-3</v>
       </c>
       <c r="D77">
@@ -3658,7 +3658,7 @@
         <v>15.3731650677034</v>
       </c>
       <c r="F77">
-        <f>POWER(10, E77-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.1265760873775839E-3</v>
       </c>
       <c r="G77">
@@ -3668,7 +3668,7 @@
         <v>16.4893292419343</v>
       </c>
       <c r="I77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.4720572580768728E-2</v>
       </c>
       <c r="J77">
@@ -3678,7 +3678,7 @@
         <v>16.6020861858599</v>
       </c>
       <c r="L77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.9084537818649685E-2</v>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
         <v>15.9795950829949</v>
       </c>
       <c r="C78">
-        <f>POWER(10, B78-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>4.5518772711153699E-3</v>
       </c>
       <c r="D78">
@@ -3700,7 +3700,7 @@
         <v>15.400093248668499</v>
       </c>
       <c r="F78">
-        <f>POWER(10, E78-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.1986398430921842E-3</v>
       </c>
       <c r="G78">
@@ -3710,7 +3710,7 @@
         <v>16.5260549290558</v>
       </c>
       <c r="I78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.6019552868014743E-2</v>
       </c>
       <c r="J78">
@@ -3720,7 +3720,7 @@
         <v>16.6386242435422</v>
       </c>
       <c r="L78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.075963457650885E-2</v>
       </c>
     </row>
@@ -3732,7 +3732,7 @@
         <v>16.022789039999001</v>
       </c>
       <c r="C79">
-        <f>POWER(10, B79-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>5.0278753358433629E-3</v>
       </c>
       <c r="D79">
@@ -3742,7 +3742,7 @@
         <v>15.4266617916811</v>
       </c>
       <c r="F79">
-        <f>POWER(10, E79-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.2742576591488835E-3</v>
       </c>
       <c r="G79">
@@ -3752,7 +3752,7 @@
         <v>16.562862413082101</v>
       </c>
       <c r="I79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.7436442183327548E-2</v>
       </c>
       <c r="J79">
@@ -3762,7 +3762,7 @@
         <v>16.675682446403801</v>
       </c>
       <c r="L79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.2608820581187156E-2</v>
       </c>
     </row>
@@ -3774,7 +3774,7 @@
         <v>16.0652524497788</v>
       </c>
       <c r="C80">
-        <f>POWER(10, B80-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>5.5443151792862345E-3</v>
       </c>
       <c r="D80">
@@ -3784,7 +3784,7 @@
         <v>15.4524611872242</v>
       </c>
       <c r="F80">
-        <f>POWER(10, E80-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.3522489354384371E-3</v>
       </c>
       <c r="G80">
@@ -3794,7 +3794,7 @@
         <v>16.598438722173601</v>
       </c>
       <c r="I80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.8924925701998118E-2</v>
       </c>
       <c r="J80">
@@ -3804,7 +3804,7 @@
         <v>16.712382475562698</v>
       </c>
       <c r="L80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.4602426133568108E-2</v>
       </c>
     </row>
@@ -3816,7 +3816,7 @@
         <v>16.1086779446034</v>
       </c>
       <c r="C81">
-        <f>POWER(10, B81-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>6.1273601194185316E-3</v>
       </c>
       <c r="D81">
@@ -3826,7 +3826,7 @@
         <v>15.4791200764318</v>
       </c>
       <c r="F81">
-        <f>POWER(10, E81-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.4378564747797114E-3</v>
       </c>
       <c r="G81">
@@ -3836,7 +3836,7 @@
         <v>16.634968752476802</v>
       </c>
       <c r="I81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.058563240970256E-2</v>
       </c>
       <c r="J81">
@@ -3846,7 +3846,7 @@
         <v>16.7500466484491</v>
       </c>
       <c r="L81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.6831324360996105E-2</v>
       </c>
     </row>
@@ -3858,7 +3858,7 @@
         <v>16.150943070310401</v>
       </c>
       <c r="C82">
-        <f>POWER(10, B82-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>6.7536497079732838E-3</v>
       </c>
       <c r="D82">
@@ -3868,7 +3868,7 @@
         <v>15.507051672031899</v>
       </c>
       <c r="F82">
-        <f>POWER(10, E82-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.5333706033353294E-3</v>
       </c>
       <c r="G82">
@@ -3878,7 +3878,7 @@
         <v>16.671579178480901</v>
       </c>
       <c r="I82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.2396215591628556E-2</v>
       </c>
       <c r="J82">
@@ -3888,7 +3888,7 @@
         <v>16.787353015703701</v>
       </c>
       <c r="L82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.9238054863523891E-2</v>
       </c>
     </row>
@@ -3900,7 +3900,7 @@
         <v>16.1941731469987</v>
       </c>
       <c r="C83">
-        <f>POWER(10, B83-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>7.4605115659540748E-3</v>
       </c>
       <c r="D83">
@@ -3910,7 +3910,7 @@
         <v>15.532575911510101</v>
       </c>
       <c r="F83">
-        <f>POWER(10, E83-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.6261903234809892E-3</v>
       </c>
       <c r="G83">
@@ -3920,7 +3920,7 @@
         <v>16.70959202025</v>
       </c>
       <c r="I83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.4444855886267849E-2</v>
       </c>
       <c r="J83">
@@ -3930,7 +3930,7 @@
         <v>16.824742473176901</v>
       </c>
       <c r="L83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.1866761806564718E-2</v>
       </c>
     </row>
@@ -3942,7 +3942,7 @@
         <v>16.237090756952199</v>
       </c>
       <c r="C84">
-        <f>POWER(10, B84-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>8.2354288213298075E-3</v>
       </c>
       <c r="D84">
@@ -3952,7 +3952,7 @@
         <v>15.5593730162119</v>
       </c>
       <c r="F84">
-        <f>POWER(10, E84-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.7296908069130276E-3</v>
       </c>
       <c r="G84">
@@ -3962,7 +3962,7 @@
         <v>16.745483498164798</v>
       </c>
       <c r="I84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.6550882401514167E-2</v>
       </c>
       <c r="J84">
@@ -3972,7 +3972,7 @@
         <v>16.8622152059305</v>
       </c>
       <c r="L84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.4738468415449961E-2</v>
       </c>
     </row>
@@ -3984,7 +3984,7 @@
         <v>16.280122106658101</v>
       </c>
       <c r="C85">
-        <f>POWER(10, B85-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>9.093217260876375E-3</v>
       </c>
       <c r="D85">
@@ -3994,7 +3994,7 @@
         <v>15.585805348825801</v>
       </c>
       <c r="F85">
-        <f>POWER(10, E85-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.838234064582204E-3</v>
       </c>
       <c r="G85">
@@ -4004,7 +4004,7 @@
         <v>16.782337146262002</v>
       </c>
       <c r="I85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.8902313485870811E-2</v>
       </c>
       <c r="J85">
@@ -4014,7 +4014,7 @@
         <v>16.8930880188279</v>
       </c>
       <c r="L85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.7297822671769808E-2</v>
       </c>
     </row>
@@ -4026,7 +4026,7 @@
         <v>16.324128409110902</v>
       </c>
       <c r="C86">
-        <f>POWER(10, B86-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.0062916525081563E-2</v>
       </c>
       <c r="D86">
@@ -4036,7 +4036,7 @@
         <v>15.6135177209521</v>
       </c>
       <c r="F86">
-        <f>POWER(10, E86-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.9593552366071782E-3</v>
       </c>
       <c r="G86">
@@ -4046,7 +4046,7 @@
         <v>16.816610968418999</v>
       </c>
       <c r="I86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.1275656123678532E-2</v>
       </c>
       <c r="J86">
@@ -4056,7 +4056,7 @@
         <v>16.923571076046201</v>
       </c>
       <c r="L86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.000981442627162E-2</v>
       </c>
     </row>
@@ -4068,7 +4068,7 @@
         <v>16.366527231853102</v>
       </c>
       <c r="C87">
-        <f>POWER(10, B87-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.109488213297165E-2</v>
       </c>
       <c r="D87">
@@ -4078,7 +4078,7 @@
         <v>15.642104309687999</v>
       </c>
       <c r="F87">
-        <f>POWER(10, E87-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.0926652887285546E-3</v>
       </c>
       <c r="G87">
@@ -4088,7 +4088,7 @@
         <v>16.850066090836901</v>
       </c>
       <c r="I87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.3780148297612514E-2</v>
       </c>
       <c r="J87">
@@ -4098,7 +4098,7 @@
         <v>16.953215003142802</v>
       </c>
       <c r="L87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.2836153300317398E-2</v>
       </c>
     </row>
@@ -4110,7 +4110,7 @@
         <v>16.410767093369401</v>
       </c>
       <c r="C88">
-        <f>POWER(10, B88-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.2284643403099784E-2</v>
       </c>
       <c r="D88">
@@ -4120,7 +4120,7 @@
         <v>15.670743237241499</v>
       </c>
       <c r="F88">
-        <f>POWER(10, E88-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.2353148239092086E-3</v>
       </c>
       <c r="G88">
@@ -4130,7 +4130,7 @@
         <v>16.8813618155793</v>
       </c>
       <c r="I88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6304233896528773E-2</v>
       </c>
       <c r="J88">
@@ -4140,7 +4140,7 @@
         <v>16.983358700718199</v>
       </c>
       <c r="L88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.5914954862110786E-2</v>
       </c>
     </row>
@@ -4152,7 +4152,7 @@
         <v>16.454258718088902</v>
       </c>
       <c r="C89">
-        <f>POWER(10, B89-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.3578574489252839E-2</v>
       </c>
       <c r="D89">
@@ -4162,7 +4162,7 @@
         <v>15.6998485988595</v>
       </c>
       <c r="F89">
-        <f>POWER(10, E89-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.3902540341704552E-3</v>
       </c>
       <c r="G89">
@@ -4172,7 +4172,7 @@
         <v>16.909148136977599</v>
       </c>
       <c r="I89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8702908032766957E-2</v>
       </c>
       <c r="J89">
@@ -4182,7 +4182,7 @@
         <v>17.0135559953548</v>
       </c>
       <c r="L89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.9221116002620247E-2</v>
       </c>
     </row>
@@ -4194,7 +4194,7 @@
         <v>16.498735723914798</v>
       </c>
       <c r="C90">
-        <f>POWER(10, B90-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.5042886714066523E-2</v>
       </c>
       <c r="D90">
@@ -4204,7 +4204,7 @@
         <v>15.728178492282501</v>
       </c>
       <c r="F90">
-        <f>POWER(10, E90-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.5513729882230313E-3</v>
       </c>
       <c r="G90">
@@ -4214,7 +4214,7 @@
         <v>16.936533571861901</v>
       </c>
       <c r="I90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.1221997522015642E-2</v>
       </c>
       <c r="J90">
@@ -4224,7 +4224,7 @@
         <v>17.044256433327799</v>
       </c>
       <c r="L90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5.2826506896448265E-2</v>
       </c>
     </row>
@@ -4236,7 +4236,7 @@
         <v>16.5415880559902</v>
       </c>
       <c r="C91">
-        <f>POWER(10, B91-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.6602883364189917E-2</v>
       </c>
       <c r="D91">
@@ -4246,7 +4246,7 @@
         <v>15.756975011949599</v>
       </c>
       <c r="F91">
-        <f>POWER(10, E91-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.7262800963485266E-3</v>
       </c>
       <c r="G91">
@@ -4256,7 +4256,7 @@
         <v>16.96396335919</v>
       </c>
       <c r="I91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.390953320141875E-2</v>
       </c>
       <c r="J91">
@@ -4266,7 +4266,7 @@
         <v>17.074562007298798</v>
       </c>
       <c r="L91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5.6644463564691862E-2</v>
       </c>
     </row>
@@ -4278,7 +4278,7 @@
         <v>16.586301119090901</v>
       </c>
       <c r="C92">
-        <f>POWER(10, B92-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.840333704798881E-2</v>
       </c>
       <c r="D92">
@@ -4288,7 +4288,7 @@
         <v>15.784991732635</v>
       </c>
       <c r="F92">
-        <f>POWER(10, E92-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.9079517324681909E-3</v>
       </c>
       <c r="G92">
@@ -4298,7 +4298,7 @@
         <v>16.9914375707936</v>
       </c>
       <c r="I92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.677707178704698E-2</v>
       </c>
       <c r="J92">
@@ -4308,7 +4308,7 @@
         <v>17.104921466155702</v>
       </c>
       <c r="L92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.0745893884001201E-2</v>
       </c>
     </row>
@@ -4320,7 +4320,7 @@
         <v>16.629819408066801</v>
       </c>
       <c r="C93">
-        <f>POWER(10, B93-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.0342993908765709E-2</v>
       </c>
       <c r="D93">
@@ -4330,7 +4330,7 @@
         <v>15.8134752642215</v>
       </c>
       <c r="F93">
-        <f>POWER(10, E93-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.105065209369132E-3</v>
       </c>
       <c r="G93">
@@ -4340,7 +4340,7 @@
         <v>17.018058722813699</v>
       </c>
       <c r="I93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.9734090901710132E-2</v>
       </c>
       <c r="J93">
@@ -4350,7 +4350,7 @@
         <v>17.135334905708699</v>
       </c>
       <c r="L93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.5152392255502165E-2</v>
       </c>
     </row>
@@ -4362,7 +4362,7 @@
         <v>16.668616112807801</v>
       </c>
       <c r="C94">
-        <f>POWER(10, B94-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.2243932770098892E-2</v>
       </c>
       <c r="D94">
@@ -4372,7 +4372,7 @@
         <v>15.842845722854801</v>
       </c>
       <c r="F94">
-        <f>POWER(10, E94-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.3223178827858943E-3</v>
       </c>
       <c r="G94">
@@ -4382,7 +4382,7 @@
         <v>17.043373229065999</v>
       </c>
       <c r="I94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.2719185278398042E-2</v>
       </c>
       <c r="J94">
@@ -4392,7 +4392,7 @@
         <v>17.166255089976001</v>
       </c>
       <c r="L94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.9960120842504941E-2</v>
       </c>
     </row>
@@ -4404,7 +4404,7 @@
         <v>16.703538608669199</v>
       </c>
       <c r="C95">
-        <f>POWER(10, B95-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.4106494977233862E-2</v>
       </c>
       <c r="D95">
@@ -4414,7 +4414,7 @@
         <v>15.8718521852793</v>
       </c>
       <c r="F95">
-        <f>POWER(10, E95-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.5517929942102157E-3</v>
       </c>
       <c r="G95">
@@ -4424,7 +4424,7 @@
         <v>17.0687253908605</v>
       </c>
       <c r="I95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.5888293864650433E-2</v>
       </c>
       <c r="J95">
@@ -4434,7 +4434,7 @@
         <v>17.196324110995398</v>
       </c>
       <c r="L95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>7.4975534752289075E-2</v>
       </c>
     </row>
@@ -4446,7 +4446,7 @@
         <v>16.7380928816237</v>
       </c>
       <c r="C96">
-        <f>POWER(10, B96-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.6102874937433844E-2</v>
       </c>
       <c r="D96">
@@ -4456,7 +4456,7 @@
         <v>15.900073163550701</v>
       </c>
       <c r="F96">
-        <f>POWER(10, E96-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.7902567037168943E-3</v>
       </c>
       <c r="G96">
@@ -4466,7 +4466,7 @@
         <v>17.09411526421</v>
       </c>
       <c r="I96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.9253052047421151E-2</v>
       </c>
       <c r="J96">
@@ -4476,7 +4476,7 @@
         <v>17.2273543484059</v>
       </c>
       <c r="L96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.052853704923231E-2</v>
       </c>
     </row>
@@ -4488,7 +4488,7 @@
         <v>16.772718636304699</v>
       </c>
       <c r="C97">
-        <f>POWER(10, B97-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.8269237680855073E-2</v>
       </c>
       <c r="D97">
@@ -4498,7 +4498,7 @@
         <v>15.926664287557299</v>
       </c>
       <c r="F97">
-        <f>POWER(10, E97-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>4.0295796866212331E-3</v>
       </c>
       <c r="G97">
@@ -4508,7 +4508,7 @@
         <v>17.1195429052108</v>
       </c>
       <c r="I97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6.2825849005588144E-2</v>
       </c>
       <c r="J97">
@@ -4518,7 +4518,7 @@
         <v>17.2552551383755</v>
       </c>
       <c r="L97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.5871806508567336E-2</v>
       </c>
     </row>
@@ -4530,7 +4530,7 @@
         <v>16.8083024668063</v>
       </c>
       <c r="C98">
-        <f>POWER(10, B98-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.0683007611160142E-2</v>
       </c>
       <c r="D98">
@@ -4540,7 +4540,7 @@
         <v>15.9537205762292</v>
       </c>
       <c r="F98">
-        <f>POWER(10, E98-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>4.2886048976280775E-3</v>
       </c>
       <c r="G98">
@@ -4550,7 +4550,7 @@
         <v>17.145008370042699</v>
       </c>
       <c r="I98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6.66198776923521E-2</v>
       </c>
       <c r="J98">
@@ -4560,7 +4560,7 @@
         <v>17.282289623731501</v>
       </c>
       <c r="L98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.1387139708775364E-2</v>
       </c>
     </row>
@@ -4572,7 +4572,7 @@
         <v>16.844405970473002</v>
       </c>
       <c r="C99">
-        <f>POWER(10, B99-10)/$N$3</f>
+        <f t="shared" ref="C99:C130" si="10">POWER(10, B99-10)/$N$3</f>
         <v>3.334275117607232E-2</v>
       </c>
       <c r="D99">
@@ -4582,7 +4582,7 @@
         <v>15.9812442479691</v>
       </c>
       <c r="F99">
-        <f>POWER(10, E99-10)/$N$3</f>
+        <f t="shared" ref="F99:F130" si="11">POWER(10, E99-10)/$N$3</f>
         <v>4.5691951691627201E-3</v>
       </c>
       <c r="G99">
@@ -4592,7 +4592,7 @@
         <v>17.170058934685201</v>
       </c>
       <c r="I99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.0575570208877184E-2</v>
       </c>
       <c r="J99">
@@ -4602,7 +4602,7 @@
         <v>17.308453593445002</v>
       </c>
       <c r="L99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.7061959449020047E-2</v>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
         <v>16.880141887824902</v>
       </c>
       <c r="C100">
-        <f>POWER(10, B100-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>3.6202398852344039E-2</v>
       </c>
       <c r="D100">
@@ -4624,7 +4624,7 @@
         <v>16.0079711216889</v>
       </c>
       <c r="F100">
-        <f>POWER(10, E100-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>4.859220230428318E-3</v>
       </c>
       <c r="G100">
@@ -4634,7 +4634,7 @@
         <v>17.1960529963361</v>
       </c>
       <c r="I100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.4928744788280127E-2</v>
       </c>
       <c r="J100">
@@ -4644,7 +4644,7 @@
         <v>17.3360285718123</v>
       </c>
       <c r="L100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.10342464355379004</v>
       </c>
     </row>
@@ -4656,7 +4656,7 @@
         <v>16.914615452263899</v>
       </c>
       <c r="C101">
-        <f>POWER(10, B101-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>3.9193217107601271E-2</v>
       </c>
       <c r="D101">
@@ -4666,7 +4666,7 @@
         <v>16.035165534774901</v>
       </c>
       <c r="F101">
-        <f>POWER(10, E101-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>5.1732205699834373E-3</v>
       </c>
       <c r="G101">
@@ -4676,7 +4676,7 @@
         <v>17.220269921557598</v>
       </c>
       <c r="I101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.9225571838671974E-2</v>
       </c>
       <c r="J101">
@@ -4686,7 +4686,7 @@
         <v>17.3622738978877</v>
       </c>
       <c r="L101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.10986752946772925</v>
       </c>
     </row>
@@ -4698,7 +4698,7 @@
         <v>16.950053342496201</v>
       </c>
       <c r="C102">
-        <f>POWER(10, B102-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>4.2525438790066275E-2</v>
       </c>
       <c r="D102">
@@ -4708,7 +4708,7 @@
         <v>16.062406145851799</v>
       </c>
       <c r="F102">
-        <f>POWER(10, E102-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>5.5080973433774879E-3</v>
       </c>
       <c r="G102">
@@ -4718,7 +4718,7 @@
         <v>17.246339998526299</v>
       </c>
       <c r="I102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.4127011124218221E-2</v>
       </c>
       <c r="J102">
@@ -4728,7 +4728,7 @@
         <v>17.389017499438602</v>
       </c>
       <c r="L102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.11684576073326353</v>
       </c>
     </row>
@@ -4740,7 +4740,7 @@
         <v>16.9855654788186</v>
       </c>
       <c r="C103">
-        <f>POWER(10, B103-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>4.614885602022685E-2</v>
       </c>
       <c r="D103">
@@ -4750,7 +4750,7 @@
         <v>16.089693033400899</v>
       </c>
       <c r="F103">
-        <f>POWER(10, E103-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>5.8652765541680734E-3</v>
       </c>
       <c r="G103">
@@ -4760,7 +4760,7 @@
         <v>17.270627742125299</v>
       </c>
       <c r="I103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.8965823504229755E-2</v>
       </c>
       <c r="J103">
@@ -4770,7 +4770,7 @@
         <v>17.417639410059198</v>
       </c>
       <c r="L103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.12480582948899949</v>
       </c>
     </row>
@@ -4782,7 +4782,7 @@
         <v>17.0220497357361</v>
       </c>
       <c r="C104">
-        <f>POWER(10, B104-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>5.019323609392564E-2</v>
       </c>
       <c r="D104">
@@ -4792,7 +4792,7 @@
         <v>16.116601275789399</v>
       </c>
       <c r="F104">
-        <f>POWER(10, E104-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>6.240174533529136E-3</v>
       </c>
       <c r="G104">
@@ -4802,7 +4802,7 @@
         <v>17.296774056706099</v>
       </c>
       <c r="I104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.4486446846763023E-2</v>
       </c>
       <c r="J104">
@@ -4812,7 +4812,7 @@
         <v>17.4444682926745</v>
       </c>
       <c r="L104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.13275893312014883</v>
       </c>
     </row>
@@ -4824,7 +4824,7 @@
         <v>17.058612359252798</v>
       </c>
       <c r="C105">
-        <f>POWER(10, B105-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>5.4601908170891979E-2</v>
       </c>
       <c r="D105">
@@ -4834,7 +4834,7 @@
         <v>16.1444059525078</v>
       </c>
       <c r="F105">
-        <f>POWER(10, E105-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>6.6527532146996322E-3</v>
       </c>
       <c r="G105">
@@ -4844,7 +4844,7 @@
         <v>17.321132825779099</v>
       </c>
       <c r="I105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.9937455283989965E-2</v>
       </c>
       <c r="J105">
@@ -4854,7 +4854,7 @@
         <v>17.474563831622302</v>
       </c>
       <c r="L105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.14228505713819584</v>
       </c>
     </row>
@@ -4866,7 +4866,7 @@
         <v>17.092999657808701</v>
       </c>
       <c r="C106">
-        <f>POWER(10, B106-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>5.910103939824693E-2</v>
       </c>
       <c r="D106">
@@ -4876,7 +4876,7 @@
         <v>16.171832141695901</v>
       </c>
       <c r="F106">
-        <f>POWER(10, E106-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>7.0864316509780872E-3</v>
       </c>
       <c r="G106">
@@ -4886,7 +4886,7 @@
         <v>17.347355600916199</v>
       </c>
       <c r="I106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.10615759277052153</v>
       </c>
       <c r="J106">
@@ -4896,7 +4896,7 @@
         <v>17.499172979179502</v>
       </c>
       <c r="L106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.15058039781880431</v>
       </c>
     </row>
@@ -4908,7 +4908,7 @@
         <v>17.129262974196301</v>
       </c>
       <c r="C107">
-        <f>POWER(10, B107-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>6.4247825773706885E-2</v>
       </c>
       <c r="D107">
@@ -4918,7 +4918,7 @@
         <v>16.196314969815301</v>
       </c>
       <c r="F107">
-        <f>POWER(10, E107-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>7.4973956657973474E-3</v>
       </c>
       <c r="G107">
@@ -4928,7 +4928,7 @@
         <v>17.371785603165399</v>
       </c>
       <c r="I107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.11230033819626797</v>
       </c>
       <c r="J107">
@@ -4938,7 +4938,7 @@
         <v>17.524278892402101</v>
       </c>
       <c r="L107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.15954175070230611</v>
       </c>
     </row>
@@ -4950,7 +4950,7 @@
         <v>17.164697934547199</v>
       </c>
       <c r="C108">
-        <f>POWER(10, B108-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>6.9709729182843239E-2</v>
       </c>
       <c r="D108">
@@ -4960,7 +4960,7 @@
         <v>16.219979398923002</v>
       </c>
       <c r="F108">
-        <f>POWER(10, E108-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>7.9172591370473347E-3</v>
       </c>
       <c r="G108">
@@ -4970,7 +4970,7 @@
         <v>17.397626281143399</v>
       </c>
       <c r="I108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.11918503878293335</v>
       </c>
       <c r="J108">
@@ -4980,7 +4980,7 @@
         <v>17.551734867830501</v>
       </c>
       <c r="L108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.16995358453036502</v>
       </c>
     </row>
@@ -4992,7 +4992,7 @@
         <v>17.201566960199401</v>
       </c>
       <c r="C109">
-        <f>POWER(10, B109-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>7.5886132745941567E-2</v>
       </c>
       <c r="D109">
@@ -5002,7 +5002,7 @@
         <v>16.2441067554326</v>
       </c>
       <c r="F109">
-        <f>POWER(10, E109-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>8.3695520856360544E-3</v>
       </c>
       <c r="G109">
@@ -5012,7 +5012,7 @@
         <v>17.4225865061901</v>
       </c>
       <c r="I109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.12623563446911712</v>
       </c>
       <c r="J109">
@@ -5022,7 +5022,7 @@
         <v>17.5773797003909</v>
       </c>
       <c r="L109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.18029146237555993</v>
       </c>
     </row>
@@ -5034,7 +5034,7 @@
         <v>17.2385151789173</v>
       </c>
       <c r="C110">
-        <f>POWER(10, B110-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>8.2624841599784907E-2</v>
       </c>
       <c r="D110">
@@ -5044,7 +5044,7 @@
         <v>16.268270001589102</v>
       </c>
       <c r="F110">
-        <f>POWER(10, E110-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>8.8484145776810512E-3</v>
       </c>
       <c r="G110">
@@ -5054,7 +5054,7 @@
         <v>17.4485027509409</v>
       </c>
       <c r="I110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.13399796779509332</v>
       </c>
       <c r="J110">
@@ -5064,7 +5064,7 @@
         <v>17.6058473785566</v>
       </c>
       <c r="L110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.1925053658987923</v>
       </c>
     </row>
@@ -5076,7 +5076,7 @@
         <v>17.273720633219799</v>
       </c>
       <c r="C111">
-        <f>POWER(10, B111-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>8.9601667951801592E-2</v>
       </c>
       <c r="D111">
@@ -5086,7 +5086,7 @@
         <v>16.292469190778501</v>
       </c>
       <c r="F111">
-        <f>POWER(10, E111-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>9.3554493480074736E-3</v>
       </c>
       <c r="G111">
@@ -5096,7 +5096,7 @@
         <v>17.473535968022102</v>
       </c>
       <c r="I111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.14194870310665331</v>
       </c>
       <c r="J111">
@@ -5106,7 +5106,7 @@
         <v>17.6329661632289</v>
       </c>
       <c r="L111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.20490927853694554</v>
       </c>
     </row>
@@ -5118,7 +5118,7 @@
         <v>17.310367354629399</v>
       </c>
       <c r="C112">
-        <f>POWER(10, B112-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>9.7490616248402995E-2</v>
       </c>
       <c r="D112">
@@ -5128,7 +5128,7 @@
         <v>16.3162741107787</v>
       </c>
       <c r="F112">
-        <f>POWER(10, E112-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>9.8825625489176623E-3</v>
       </c>
       <c r="G112">
@@ -5138,7 +5138,7 @@
         <v>17.500912442519599</v>
       </c>
       <c r="I112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.15118472124690049</v>
       </c>
       <c r="J112">
@@ -5148,7 +5148,7 @@
         <v>17.660126719732201</v>
       </c>
       <c r="L112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.21813340605165038</v>
       </c>
     </row>
@@ -5160,7 +5160,7 @@
         <v>17.343432667793699</v>
       </c>
       <c r="C113">
-        <f>POWER(10, B113-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.10520300104634855</v>
       </c>
       <c r="D113">
@@ -5170,7 +5170,7 @@
         <v>16.3409756121981</v>
       </c>
       <c r="F113">
-        <f>POWER(10, E113-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.046094872041365E-2</v>
       </c>
       <c r="G113">
@@ -5180,7 +5180,7 @@
         <v>17.524634423096799</v>
       </c>
       <c r="I113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.15967241138439525</v>
       </c>
       <c r="J113">
@@ -5190,7 +5190,7 @@
         <v>17.6887284119295</v>
       </c>
       <c r="L113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.23298280675096639</v>
       </c>
     </row>
@@ -5202,7 +5202,7 @@
         <v>17.370605304345201</v>
       </c>
       <c r="C114">
-        <f>POWER(10, B114-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.11199554960255048</v>
       </c>
       <c r="D114">
@@ -5212,7 +5212,7 @@
         <v>16.364851404910599</v>
       </c>
       <c r="F114">
-        <f>POWER(10, E114-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.1052152426855194E-2</v>
       </c>
       <c r="G114">
@@ -5222,7 +5222,7 @@
         <v>17.5497768656343</v>
       </c>
       <c r="I114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.16918907912775349</v>
       </c>
       <c r="J114">
@@ -5232,7 +5232,7 @@
         <v>17.715974860601602</v>
       </c>
       <c r="L114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.24806775800851075</v>
       </c>
     </row>
@@ -5244,7 +5244,7 @@
         <v>17.3969029767592</v>
       </c>
       <c r="C115">
-        <f>POWER(10, B115-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.11898670489457835</v>
       </c>
       <c r="D115">
@@ -5254,7 +5254,7 @@
         <v>16.389194259754099</v>
       </c>
       <c r="F115">
-        <f>POWER(10, E115-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.1689332729937928E-2</v>
       </c>
       <c r="G115">
@@ -5264,7 +5264,7 @@
         <v>17.574955379818199</v>
       </c>
       <c r="I115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17928784239106191</v>
       </c>
       <c r="J115">
@@ -5274,7 +5274,7 @@
         <v>17.702992432412099</v>
       </c>
       <c r="L115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.24076197287364265</v>
       </c>
     </row>
@@ -5286,7 +5286,7 @@
         <v>17.4236999184597</v>
       </c>
       <c r="C116">
-        <f>POWER(10, B116-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.12655968331855597</v>
       </c>
       <c r="D116">
@@ -5296,7 +5296,7 @@
         <v>16.414871853545598</v>
       </c>
       <c r="F116">
-        <f>POWER(10, E116-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.2401302880843392E-2</v>
       </c>
       <c r="G116">
@@ -5306,7 +5306,7 @@
         <v>17.591124237289499</v>
       </c>
       <c r="I116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.18608856988178557</v>
       </c>
     </row>
@@ -5318,7 +5318,7 @@
         <v>17.450538136247498</v>
       </c>
       <c r="C117">
-        <f>POWER(10, B117-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.13462744299695942</v>
       </c>
       <c r="D117">
@@ -5328,7 +5328,7 @@
         <v>16.441890343523902</v>
       </c>
       <c r="F117">
-        <f>POWER(10, E117-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.3197321738226667E-2</v>
       </c>
     </row>
@@ -5340,7 +5340,7 @@
         <v>17.476956820416198</v>
       </c>
       <c r="C118">
-        <f>POWER(10, B118-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.14307122030048897</v>
       </c>
       <c r="D118">
@@ -5350,7 +5350,7 @@
         <v>16.468519024858299</v>
       </c>
       <c r="F118">
-        <f>POWER(10, E118-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.4031835538111742E-2</v>
       </c>
     </row>
@@ -5362,7 +5362,7 @@
         <v>17.5038770713163</v>
       </c>
       <c r="C119">
-        <f>POWER(10, B119-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.15222028555273115</v>
       </c>
       <c r="D119">
@@ -5372,7 +5372,7 @@
         <v>16.496060812062201</v>
       </c>
       <c r="F119">
-        <f>POWER(10, E119-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.495051913111653E-2</v>
       </c>
     </row>
@@ -5384,7 +5384,7 @@
         <v>17.530376506260001</v>
       </c>
       <c r="C120">
-        <f>POWER(10, B120-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.16179755975217205</v>
       </c>
       <c r="D120">
@@ -5394,7 +5394,7 @@
         <v>16.522777225896601</v>
       </c>
       <c r="F120">
-        <f>POWER(10, E120-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.5899105343784057E-2</v>
       </c>
     </row>
@@ -5406,7 +5406,7 @@
         <v>17.557842035059402</v>
       </c>
       <c r="C121">
-        <f>POWER(10, B121-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.17236040109423761</v>
       </c>
       <c r="D121">
@@ -5416,7 +5416,7 @@
         <v>16.550409753975501</v>
       </c>
       <c r="F121">
-        <f>POWER(10, E121-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.6943581460136036E-2</v>
       </c>
     </row>
@@ -5428,7 +5428,7 @@
         <v>17.583959473553001</v>
       </c>
       <c r="C122">
-        <f>POWER(10, B122-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.18304376263978656</v>
       </c>
       <c r="D122">
@@ -5438,7 +5438,7 @@
         <v>16.577214189358799</v>
       </c>
       <c r="F122">
-        <f>POWER(10, E122-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.80222765807036E-2</v>
       </c>
     </row>
@@ -5450,7 +5450,7 @@
         <v>17.611508952889899</v>
       </c>
       <c r="C123">
-        <f>POWER(10, B123-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.19503134413510831</v>
       </c>
       <c r="D123">
@@ -5460,7 +5460,7 @@
         <v>16.604062036220601</v>
       </c>
       <c r="F123">
-        <f>POWER(10, E123-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.9171561947773894E-2</v>
       </c>
     </row>
@@ -5472,7 +5472,7 @@
         <v>17.637706221377599</v>
       </c>
       <c r="C124">
-        <f>POWER(10, B124-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.2071579870655274</v>
       </c>
       <c r="D124">
@@ -5482,7 +5482,7 @@
         <v>16.623937915284699</v>
       </c>
       <c r="F124">
-        <f>POWER(10, E124-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.0069353205106527E-2</v>
       </c>
     </row>
@@ -5494,7 +5494,7 @@
         <v>17.6653399078535</v>
       </c>
       <c r="C125">
-        <f>POWER(10, B125-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.22076761649940962</v>
       </c>
       <c r="D125">
@@ -5504,7 +5504,7 @@
         <v>16.6433986946797</v>
       </c>
       <c r="F125">
-        <f>POWER(10, E125-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.098911638239867E-2</v>
       </c>
     </row>
@@ -5516,7 +5516,7 @@
         <v>17.692083784295299</v>
       </c>
       <c r="C126">
-        <f>POWER(10, B126-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.23478981049083331</v>
       </c>
       <c r="D126">
@@ -5526,7 +5526,7 @@
         <v>16.661564107730499</v>
       </c>
       <c r="F126">
-        <f>POWER(10, E126-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.1885656002367367E-2</v>
       </c>
     </row>
@@ -5538,7 +5538,7 @@
         <v>17.719335401342398</v>
       </c>
       <c r="C127">
-        <f>POWER(10, B127-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.24999473499943231</v>
       </c>
       <c r="D127">
@@ -5548,7 +5548,7 @@
         <v>16.6793095083402</v>
       </c>
       <c r="F127">
-        <f>POWER(10, E127-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.2798431507960952E-2</v>
       </c>
     </row>
@@ -5560,7 +5560,7 @@
         <v>17.7461610225348</v>
       </c>
       <c r="C128">
-        <f>POWER(10, B128-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.2659233563142549</v>
       </c>
       <c r="D128">
@@ -5570,7 +5570,7 @@
         <v>16.6970738086907</v>
       </c>
       <c r="F128">
-        <f>POWER(10, E128-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.3750309292977379E-2</v>
       </c>
     </row>
@@ -5582,7 +5582,7 @@
         <v>17.773964629403601</v>
       </c>
       <c r="C129">
-        <f>POWER(10, B129-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.28350458725022554</v>
       </c>
       <c r="D129">
@@ -5592,7 +5592,7 @@
         <v>16.7152978053659</v>
       </c>
       <c r="F129">
-        <f>POWER(10, E129-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.4768132730329701E-2</v>
       </c>
     </row>
@@ -5604,7 +5604,7 @@
         <v>17.8004035520839</v>
       </c>
       <c r="C130">
-        <f>POWER(10, B130-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.30129991771978143</v>
       </c>
       <c r="D130">
@@ -5614,7 +5614,7 @@
         <v>16.734865535031901</v>
       </c>
       <c r="F130">
-        <f>POWER(10, E130-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.5909617166923485E-2</v>
       </c>
     </row>
@@ -5626,7 +5626,7 @@
         <v>17.828292142852298</v>
       </c>
       <c r="C131">
-        <f>POWER(10, B131-10)/$N$3</f>
+        <f t="shared" ref="C131:C162" si="12">POWER(10, B131-10)/$N$3</f>
         <v>0.32128289453919295</v>
       </c>
       <c r="D131">
@@ -5636,7 +5636,7 @@
         <v>16.761084705575101</v>
       </c>
       <c r="F131">
-        <f>POWER(10, E131-10)/$N$3</f>
+        <f t="shared" ref="F131:F162" si="13">POWER(10, E131-10)/$N$3</f>
         <v>2.7522011156600055E-2</v>
       </c>
     </row>
@@ -5648,7 +5648,7 @@
         <v>17.854811878168199</v>
       </c>
       <c r="C132">
-        <f>POWER(10, B132-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.3415130778623866</v>
       </c>
       <c r="D132">
@@ -5658,7 +5658,7 @@
         <v>16.788673053701402</v>
       </c>
       <c r="F132">
-        <f>POWER(10, E132-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>2.932705912158317E-2</v>
       </c>
     </row>
@@ -5670,7 +5670,7 @@
         <v>17.8827857125961</v>
       </c>
       <c r="C133">
-        <f>POWER(10, B133-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.36423457896525047</v>
       </c>
       <c r="D133">
@@ -5680,7 +5680,7 @@
         <v>16.8163068115946</v>
       </c>
       <c r="F133">
-        <f>POWER(10, E133-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.1253759981027626E-2</v>
       </c>
     </row>
@@ -5692,7 +5692,7 @@
         <v>17.909858784160399</v>
       </c>
       <c r="C134">
-        <f>POWER(10, B134-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.38766290435324507</v>
       </c>
       <c r="D134">
@@ -5702,7 +5702,7 @@
         <v>16.843541884080398</v>
       </c>
       <c r="F134">
-        <f>POWER(10, E134-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.3276477308652588E-2</v>
       </c>
     </row>
@@ -5714,7 +5714,7 @@
         <v>17.937445846199299</v>
       </c>
       <c r="C135">
-        <f>POWER(10, B135-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.41308679017760908</v>
       </c>
       <c r="D135">
@@ -5724,7 +5724,7 @@
         <v>16.869486468038801</v>
       </c>
       <c r="F135">
-        <f>POWER(10, E135-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.5324980357393149E-2</v>
       </c>
     </row>
@@ -5736,7 +5736,7 @@
         <v>17.964601668724899</v>
       </c>
       <c r="C136">
-        <f>POWER(10, B136-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.43974117215563574</v>
       </c>
       <c r="D136">
@@ -5746,7 +5746,7 @@
         <v>16.8972532428965</v>
       </c>
       <c r="F136">
-        <f>POWER(10, E136-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.765725887187199E-2</v>
       </c>
     </row>
@@ -5758,7 +5758,7 @@
         <v>17.992273052777101</v>
       </c>
       <c r="C137">
-        <f>POWER(10, B137-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.46867146651563363</v>
       </c>
       <c r="D137">
@@ -5768,7 +5768,7 @@
         <v>16.917514761469299</v>
       </c>
       <c r="F137">
-        <f>POWER(10, E137-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.945574266997235E-2</v>
       </c>
     </row>
@@ -5780,7 +5780,7 @@
         <v>18.019987059844901</v>
       </c>
       <c r="C138">
-        <f>POWER(10, B138-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.49955409208607204</v>
       </c>
       <c r="D138">
@@ -5790,7 +5790,7 @@
         <v>16.691477043366401</v>
       </c>
       <c r="F138">
-        <f>POWER(10, E138-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>2.3446202110167215E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating IceCube acceptances, tau_Shower_sim_GEOM for Steph's environment
</commit_message>
<xml_diff>
--- a/util/icecube_acceptance.xlsx
+++ b/util/icecube_acceptance.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wissels/nutau_acceptance/util/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wissels/Library/Caches/com.binarynights.ForkLift2/#25/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31000" yWindow="10200" windowWidth="24160" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="540" yWindow="5300" windowWidth="34960" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="icecube_acceptance.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -460,12 +460,23 @@
   <dimension ref="A1:N141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -531,7 +542,7 @@
         <v>11.979551673969199</v>
       </c>
       <c r="C3">
-        <f>POWER(10, B3-10)/$N$3</f>
+        <f t="shared" ref="C3:C34" si="0">POWER(10, B3-10)/$N$3</f>
         <v>4.5514223201753288E-7</v>
       </c>
       <c r="D3">
@@ -541,7 +552,7 @@
         <v>12.020664990976</v>
       </c>
       <c r="F3">
-        <f>POWER(10, E3-10)/$N$3</f>
+        <f t="shared" ref="F3:F34" si="1">POWER(10, E3-10)/$N$3</f>
         <v>5.0033450203391288E-7</v>
       </c>
       <c r="G3">
@@ -551,7 +562,7 @@
         <v>12.013846700824001</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="0">POWER(10, H3-10)/$N$3</f>
+        <f t="shared" ref="I3:I66" si="2">POWER(10, H3-10)/$N$3</f>
         <v>4.9254074371361153E-7</v>
       </c>
       <c r="J3">
@@ -561,7 +572,7 @@
         <v>12.023877872285</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L66" si="1">POWER(10, K3-10)/$N$3</f>
+        <f t="shared" ref="L3:L66" si="3">POWER(10, K3-10)/$N$3</f>
         <v>5.0404966829199579E-7</v>
       </c>
       <c r="M3">
@@ -579,7 +590,7 @@
         <v>12.3116347673402</v>
       </c>
       <c r="C4">
-        <f>POWER(10, B4-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>9.777554116059838E-7</v>
       </c>
       <c r="D4">
@@ -589,7 +600,7 @@
         <v>12.3339875579512</v>
       </c>
       <c r="F4">
-        <f>POWER(10, E4-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.0293972860971493E-6</v>
       </c>
       <c r="G4">
@@ -599,7 +610,7 @@
         <v>12.104843423721601</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0734978867375655E-7</v>
       </c>
       <c r="J4">
@@ -609,7 +620,7 @@
         <v>12.112287538826299</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.1784992716697401E-7</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -624,7 +635,7 @@
         <v>12.195446336726199</v>
       </c>
       <c r="C5">
-        <f>POWER(10, B5-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>7.4824150990353195E-7</v>
       </c>
       <c r="D5">
@@ -634,7 +645,7 @@
         <v>12.208767664360799</v>
       </c>
       <c r="F5">
-        <f>POWER(10, E5-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>7.7154831183309275E-7</v>
       </c>
       <c r="G5">
@@ -644,7 +655,7 @@
         <v>12.199177688552099</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5469791390990651E-7</v>
       </c>
       <c r="J5">
@@ -654,7 +665,7 @@
         <v>12.1934824667513</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4486561706870449E-7</v>
       </c>
     </row>
@@ -666,7 +677,7 @@
         <v>12.118307815306601</v>
       </c>
       <c r="C6">
-        <f>POWER(10, B6-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>6.2647432418291061E-7</v>
       </c>
       <c r="D6">
@@ -676,7 +687,7 @@
         <v>12.4340361389494</v>
       </c>
       <c r="F6">
-        <f>POWER(10, E6-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.2960793760695447E-6</v>
       </c>
       <c r="G6">
@@ -686,7 +697,7 @@
         <v>12.2874786219946</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.2485592460533784E-7</v>
       </c>
       <c r="J6">
@@ -696,7 +707,7 @@
         <v>12.277680993867</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.042248847074522E-7</v>
       </c>
     </row>
@@ -708,7 +719,7 @@
         <v>12.037161848442199</v>
       </c>
       <c r="C7">
-        <f>POWER(10, B7-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>5.1970549579163583E-7</v>
       </c>
       <c r="D7">
@@ -718,7 +729,7 @@
         <v>12.5122413616345</v>
       </c>
       <c r="F7">
-        <f>POWER(10, E7-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.551803841474921E-6</v>
       </c>
       <c r="G7">
@@ -728,7 +739,7 @@
         <v>12.369784378528101</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1178404979833432E-6</v>
       </c>
       <c r="J7">
@@ -738,7 +749,7 @@
         <v>12.3703933908424</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.119409148309624E-6</v>
       </c>
     </row>
@@ -750,7 +761,7 @@
         <v>11.966119912668701</v>
       </c>
       <c r="C8">
-        <f>POWER(10, B8-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>4.4128114732730155E-7</v>
       </c>
       <c r="D8">
@@ -760,7 +771,7 @@
         <v>12.5950839083325</v>
       </c>
       <c r="F8">
-        <f>POWER(10, E8-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.8779298679201243E-6</v>
       </c>
       <c r="G8">
@@ -770,7 +781,7 @@
         <v>12.451919040955699</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3505619250189747E-6</v>
       </c>
       <c r="J8">
@@ -780,7 +791,7 @@
         <v>12.455969552247799</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3632170625017857E-6</v>
       </c>
     </row>
@@ -792,7 +803,7 @@
         <v>12.436323171848599</v>
       </c>
       <c r="C9">
-        <f>POWER(10, B9-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.3029226467563407E-6</v>
       </c>
       <c r="D9">
@@ -802,7 +813,7 @@
         <v>12.683446323462199</v>
       </c>
       <c r="F9">
-        <f>POWER(10, E9-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.3016632549748102E-6</v>
       </c>
       <c r="G9">
@@ -812,7 +823,7 @@
         <v>12.5345990728551</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.6337836059043367E-6</v>
       </c>
       <c r="J9">
@@ -822,7 +833,7 @@
         <v>12.5365986066553</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6413230464861584E-6</v>
       </c>
     </row>
@@ -834,7 +845,7 @@
         <v>12.5335254495035</v>
       </c>
       <c r="C10">
-        <f>POWER(10, B10-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.6297497027229012E-6</v>
       </c>
       <c r="D10">
@@ -844,7 +855,7 @@
         <v>12.7705763420811</v>
       </c>
       <c r="F10">
-        <f>POWER(10, E10-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.8130134136489863E-6</v>
       </c>
       <c r="G10">
@@ -854,7 +865,7 @@
         <v>12.6260825737084</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0168705972401809E-6</v>
       </c>
       <c r="J10">
@@ -864,7 +875,7 @@
         <v>12.619607193385599</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9870219029967818E-6</v>
       </c>
     </row>
@@ -876,7 +887,7 @@
         <v>12.6363854378368</v>
       </c>
       <c r="C11">
-        <f>POWER(10, B11-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.0652893181024261E-6</v>
       </c>
       <c r="D11">
@@ -886,7 +897,7 @@
         <v>12.856750915327</v>
       </c>
       <c r="F11">
-        <f>POWER(10, E11-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.4304127379320456E-6</v>
       </c>
       <c r="G11">
@@ -896,7 +907,7 @@
         <v>12.7027318824865</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4061757384654503E-6</v>
       </c>
       <c r="J11">
@@ -906,7 +917,7 @@
         <v>12.7018387936014</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.4012327312016271E-6</v>
       </c>
     </row>
@@ -918,7 +929,7 @@
         <v>12.744235340094001</v>
       </c>
       <c r="C12">
-        <f>POWER(10, B12-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.6474684974329554E-6</v>
       </c>
       <c r="D12">
@@ -928,7 +939,7 @@
         <v>12.9438198665905</v>
       </c>
       <c r="F12">
-        <f>POWER(10, E12-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>4.1919426031952488E-6</v>
       </c>
       <c r="G12">
@@ -938,7 +949,7 @@
         <v>12.7898134756384</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.940417079037278E-6</v>
       </c>
       <c r="J12">
@@ -948,7 +959,7 @@
         <v>12.781368887970499</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8837947639929699E-6</v>
       </c>
     </row>
@@ -960,7 +971,7 @@
         <v>12.830710967669599</v>
       </c>
       <c r="C13">
-        <f>POWER(10, B13-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.2307728801741338E-6</v>
       </c>
       <c r="D13">
@@ -970,7 +981,7 @@
         <v>13.028958686460401</v>
       </c>
       <c r="F13">
-        <f>POWER(10, E13-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>5.0998117761230631E-6</v>
       </c>
       <c r="G13">
@@ -980,7 +991,7 @@
         <v>12.8818301312457</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6343403198349643E-6</v>
       </c>
       <c r="J13">
@@ -990,7 +1001,7 @@
         <v>12.8681551788903</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5216860731273602E-6</v>
       </c>
     </row>
@@ -1002,7 +1013,7 @@
         <v>12.915730202065101</v>
       </c>
       <c r="C14">
-        <f>POWER(10, B14-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.9293947725883628E-6</v>
       </c>
       <c r="D14">
@@ -1012,7 +1023,7 @@
         <v>13.1148897257097</v>
       </c>
       <c r="F14">
-        <f>POWER(10, E14-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>6.215630465696085E-6</v>
       </c>
       <c r="G14">
@@ -1022,7 +1033,7 @@
         <v>12.964462600757299</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.396003826143235E-6</v>
       </c>
       <c r="J14">
@@ -1032,7 +1043,7 @@
         <v>12.955396540196601</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3051868114834216E-6</v>
       </c>
     </row>
@@ -1044,7 +1055,7 @@
         <v>13.0041415683284</v>
       </c>
       <c r="C15">
-        <f>POWER(10, B15-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>4.8165606060603615E-6</v>
       </c>
       <c r="D15">
@@ -1054,7 +1065,7 @@
         <v>13.206864925030199</v>
       </c>
       <c r="F15">
-        <f>POWER(10, E15-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>7.6817538370536299E-6</v>
       </c>
       <c r="G15">
@@ -1064,7 +1075,7 @@
         <v>13.0478110982649</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.3260661887594399E-6</v>
       </c>
       <c r="J15">
@@ -1074,7 +1085,7 @@
         <v>13.0390160925283</v>
       </c>
       <c r="L15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2192915051122168E-6</v>
       </c>
     </row>
@@ -1086,7 +1097,7 @@
         <v>13.0909428598091</v>
       </c>
       <c r="C16">
-        <f>POWER(10, B16-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>5.8821801438855626E-6</v>
       </c>
       <c r="D16">
@@ -1096,7 +1107,7 @@
         <v>13.299485149773499</v>
       </c>
       <c r="F16">
-        <f>POWER(10, E16-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>9.507812547766368E-6</v>
       </c>
       <c r="G16">
@@ -1106,7 +1117,7 @@
         <v>13.1322396128592</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.4689690579498688E-6</v>
       </c>
       <c r="J16">
@@ -1116,7 +1127,7 @@
         <v>13.119049040793501</v>
       </c>
       <c r="L16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.2754446264764857E-6</v>
       </c>
     </row>
@@ -1128,7 +1139,7 @@
         <v>13.179785664592799</v>
       </c>
       <c r="C17">
-        <f>POWER(10, B17-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>7.2174058217717719E-6</v>
       </c>
       <c r="D17">
@@ -1138,7 +1149,7 @@
         <v>13.3867086173784</v>
       </c>
       <c r="F17">
-        <f>POWER(10, E17-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.1622621057981298E-5</v>
       </c>
       <c r="G17">
@@ -1148,7 +1159,7 @@
         <v>13.216392911383601</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.8521461130833756E-6</v>
       </c>
       <c r="J17">
@@ -1158,7 +1169,7 @@
         <v>13.1972862360757</v>
       </c>
       <c r="L17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.5141817789278837E-6</v>
       </c>
     </row>
@@ -1170,7 +1181,7 @@
         <v>13.2691914279293</v>
       </c>
       <c r="C18">
-        <f>POWER(10, B18-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>8.8672078570124654E-6</v>
       </c>
       <c r="D18">
@@ -1180,7 +1191,7 @@
         <v>13.469132668625999</v>
       </c>
       <c r="F18">
-        <f>POWER(10, E18-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.4051676072272072E-5</v>
       </c>
       <c r="G18">
@@ -1190,7 +1201,7 @@
         <v>13.301085476465801</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.5429124056088258E-6</v>
       </c>
       <c r="J18">
@@ -1200,7 +1211,7 @@
         <v>13.285638974969601</v>
       </c>
       <c r="L18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.2094657261391616E-6</v>
       </c>
     </row>
@@ -1212,7 +1223,7 @@
         <v>13.3580965535137</v>
       </c>
       <c r="C19">
-        <f>POWER(10, B19-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.0881581383602971E-5</v>
       </c>
       <c r="D19">
@@ -1222,7 +1233,7 @@
         <v>13.554965265239501</v>
       </c>
       <c r="F19">
-        <f>POWER(10, E19-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.7122245757253025E-5</v>
       </c>
       <c r="G19">
@@ -1232,7 +1243,7 @@
         <v>13.386320763804299</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1612245925461964E-5</v>
       </c>
       <c r="J19">
@@ -1242,7 +1253,7 @@
         <v>13.3697622487087</v>
       </c>
       <c r="L19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1177835389863527E-5</v>
       </c>
     </row>
@@ -1254,7 +1265,7 @@
         <v>13.4475973537778</v>
       </c>
       <c r="C20">
-        <f>POWER(10, B20-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.3371890598295518E-5</v>
       </c>
       <c r="D20">
@@ -1264,7 +1275,7 @@
         <v>13.6408502245799</v>
       </c>
       <c r="F20">
-        <f>POWER(10, E20-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.0866311460010096E-5</v>
       </c>
       <c r="G20">
@@ -1274,7 +1285,7 @@
         <v>13.470985768511699</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4111761551172588E-5</v>
       </c>
       <c r="J20">
@@ -1284,7 +1295,7 @@
         <v>13.4544181822016</v>
       </c>
       <c r="L20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3583561181457722E-5</v>
       </c>
     </row>
@@ -1296,7 +1307,7 @@
         <v>13.537697819811401</v>
       </c>
       <c r="C21">
-        <f>POWER(10, B21-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.6454825490517985E-5</v>
       </c>
       <c r="D21">
@@ -1306,7 +1317,7 @@
         <v>13.729020023658901</v>
       </c>
       <c r="F21">
-        <f>POWER(10, E21-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.5563215704251914E-5</v>
       </c>
       <c r="G21">
@@ -1316,7 +1327,7 @@
         <v>13.5539334823495</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7081615558449263E-5</v>
       </c>
       <c r="J21">
@@ -1326,7 +1337,7 @@
         <v>13.548645066438899</v>
       </c>
       <c r="L21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6874873559787811E-5</v>
       </c>
     </row>
@@ -1338,7 +1349,7 @@
         <v>13.627272533581101</v>
       </c>
       <c r="C22">
-        <f>POWER(10, B22-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.0224043678917554E-5</v>
       </c>
       <c r="D22">
@@ -1348,7 +1359,7 @@
         <v>13.830055250997599</v>
       </c>
       <c r="F22">
-        <f>POWER(10, E22-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.2258985995799319E-5</v>
       </c>
       <c r="G22">
@@ -1358,7 +1369,7 @@
         <v>13.6364119880323</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0654155815333156E-5</v>
       </c>
       <c r="J22">
@@ -1368,7 +1379,7 @@
         <v>13.631548087440301</v>
       </c>
       <c r="L22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.0424129169137591E-5</v>
       </c>
     </row>
@@ -1380,7 +1391,7 @@
         <v>13.7129516753619</v>
       </c>
       <c r="C23">
-        <f>POWER(10, B23-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.4634691974946078E-5</v>
       </c>
       <c r="D23">
@@ -1390,7 +1401,7 @@
         <v>13.9191268854527</v>
       </c>
       <c r="F23">
-        <f>POWER(10, E23-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.9602476637812306E-5</v>
       </c>
       <c r="G23">
@@ -1400,7 +1411,7 @@
         <v>13.7302609210961</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5636361211740782E-5</v>
       </c>
       <c r="J23">
@@ -1410,7 +1421,7 @@
         <v>13.718545357983899</v>
       </c>
       <c r="L23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.4954037246249327E-5</v>
       </c>
     </row>
@@ -1422,7 +1433,7 @@
         <v>13.7985361673336</v>
       </c>
       <c r="C24">
-        <f>POWER(10, B24-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.0000716591770054E-5</v>
       </c>
       <c r="D24">
@@ -1432,7 +1443,7 @@
         <v>14.0079594992993</v>
       </c>
       <c r="F24">
-        <f>POWER(10, E24-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>4.8590901919467273E-5</v>
       </c>
       <c r="G24">
@@ -1442,7 +1453,7 @@
         <v>13.8169428417792</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1299565071153124E-5</v>
       </c>
       <c r="J24">
@@ -1452,7 +1463,7 @@
         <v>13.804095628190201</v>
       </c>
       <c r="L24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.038722833150881E-5</v>
       </c>
     </row>
@@ -1464,7 +1475,7 @@
         <v>13.889221708320701</v>
       </c>
       <c r="C25">
-        <f>POWER(10, B25-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>3.6967252109001644E-5</v>
       </c>
       <c r="D25">
@@ -1474,7 +1485,7 @@
         <v>14.0944968844692</v>
       </c>
       <c r="F25">
-        <f>POWER(10, E25-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>5.9305141364087674E-5</v>
       </c>
       <c r="G25">
@@ -1484,7 +1495,7 @@
         <v>13.9041720030003</v>
       </c>
       <c r="I25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.826198208191486E-5</v>
       </c>
       <c r="J25">
@@ -1494,7 +1505,7 @@
         <v>13.888158870177501</v>
       </c>
       <c r="L25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.6876893678381349E-5</v>
       </c>
     </row>
@@ -1506,7 +1517,7 @@
         <v>13.980052660725599</v>
       </c>
       <c r="C26">
-        <f>POWER(10, B26-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>4.5566757094917849E-5</v>
       </c>
       <c r="D26">
@@ -1516,7 +1527,7 @@
         <v>14.181974002371399</v>
       </c>
       <c r="F26">
-        <f>POWER(10, E26-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>7.2538649097431921E-5</v>
       </c>
       <c r="G26">
@@ -1526,7 +1537,7 @@
         <v>13.991951859599901</v>
       </c>
       <c r="I26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.6832497713620888E-5</v>
       </c>
       <c r="J26">
@@ -1536,7 +1547,7 @@
         <v>13.975983018544101</v>
       </c>
       <c r="L26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.5141759175100172E-5</v>
       </c>
     </row>
@@ -1548,7 +1559,7 @@
         <v>14.0753898023933</v>
       </c>
       <c r="C27">
-        <f>POWER(10, B27-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>5.6752534763427918E-5</v>
       </c>
       <c r="D27">
@@ -1558,7 +1569,7 @@
         <v>14.2655606790701</v>
       </c>
       <c r="F27">
-        <f>POWER(10, E27-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>8.7933860490093852E-5</v>
       </c>
       <c r="G27">
@@ -1568,7 +1579,7 @@
         <v>14.079947602579599</v>
       </c>
       <c r="I27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.7351273183520524E-5</v>
       </c>
       <c r="J27">
@@ -1578,7 +1589,7 @@
         <v>14.0639545790157</v>
       </c>
       <c r="L27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5277709601091373E-5</v>
       </c>
     </row>
@@ -1590,7 +1601,7 @@
         <v>14.1693581360419</v>
       </c>
       <c r="C28">
-        <f>POWER(10, B28-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>7.0461777880322047E-5</v>
       </c>
       <c r="D28">
@@ -1600,7 +1611,7 @@
         <v>14.3373535873267</v>
       </c>
       <c r="F28">
-        <f>POWER(10, E28-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.0374066995172044E-4</v>
       </c>
       <c r="G28">
@@ -1610,7 +1621,7 @@
         <v>14.164464294762301</v>
       </c>
       <c r="I28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.9672237143221868E-5</v>
       </c>
       <c r="J28">
@@ -1620,7 +1631,7 @@
         <v>14.153151652153401</v>
       </c>
       <c r="L28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.7880825187836594E-5</v>
       </c>
     </row>
@@ -1632,7 +1643,7 @@
         <v>14.2699682918619</v>
       </c>
       <c r="C29">
-        <f>POWER(10, B29-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>8.8830836719025718E-5</v>
       </c>
       <c r="D29">
@@ -1642,7 +1653,7 @@
         <v>14.4068481960689</v>
       </c>
       <c r="F29">
-        <f>POWER(10, E29-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.2174290401552009E-4</v>
       </c>
       <c r="G29">
@@ -1652,7 +1663,7 @@
         <v>14.230118589989299</v>
       </c>
       <c r="I29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1042727903695246E-5</v>
       </c>
       <c r="J29">
@@ -1662,7 +1673,7 @@
         <v>14.2341347099907</v>
       </c>
       <c r="L29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.1795643040075301E-5</v>
       </c>
     </row>
@@ -1674,7 +1685,7 @@
         <v>14.3593674882838</v>
       </c>
       <c r="C30">
-        <f>POWER(10, B30-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.0913472269729516E-4</v>
       </c>
       <c r="D30">
@@ -1684,7 +1695,7 @@
         <v>14.4774431722184</v>
       </c>
       <c r="F30">
-        <f>POWER(10, E30-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.4323153070066073E-4</v>
       </c>
       <c r="G30">
@@ -1694,7 +1705,7 @@
         <v>14.295700219691501</v>
       </c>
       <c r="I30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.4253108149795441E-5</v>
       </c>
       <c r="J30">
@@ -1704,7 +1715,7 @@
         <v>14.3046377795037</v>
       </c>
       <c r="L30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.6212885681270382E-5</v>
       </c>
     </row>
@@ -1716,7 +1727,7 @@
         <v>14.449745894741101</v>
       </c>
       <c r="C31">
-        <f>POWER(10, B31-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.3438207901154002E-4</v>
       </c>
       <c r="D31">
@@ -1726,7 +1737,7 @@
         <v>14.547937563950001</v>
       </c>
       <c r="F31">
-        <f>POWER(10, E31-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>1.6847405341825276E-4</v>
       </c>
       <c r="G31">
@@ -1736,7 +1747,7 @@
         <v>14.361962811990701</v>
       </c>
       <c r="I31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0978885934334265E-4</v>
       </c>
       <c r="J31">
@@ -1746,7 +1757,7 @@
         <v>14.3751109810988</v>
       </c>
       <c r="L31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1316351848283813E-4</v>
       </c>
     </row>
@@ -1758,7 +1769,7 @@
         <v>14.543537265678101</v>
       </c>
       <c r="C32">
-        <f>POWER(10, B32-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.6677568252572821E-4</v>
       </c>
       <c r="D32">
@@ -1768,7 +1779,7 @@
         <v>14.6588509468884</v>
       </c>
       <c r="F32">
-        <f>POWER(10, E32-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.1749356294912167E-4</v>
       </c>
       <c r="G32">
@@ -1778,7 +1789,7 @@
         <v>14.4285325407764</v>
       </c>
       <c r="I32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.279758438130177E-4</v>
       </c>
       <c r="J32">
@@ -1788,7 +1799,7 @@
         <v>14.4463123199512</v>
       </c>
       <c r="L32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3332382993118492E-4</v>
       </c>
     </row>
@@ -1800,7 +1811,7 @@
         <v>14.6144166446126</v>
       </c>
       <c r="C33">
-        <f>POWER(10, B33-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>1.963415004659225E-4</v>
       </c>
       <c r="D33">
@@ -1810,7 +1821,7 @@
         <v>14.783185633839301</v>
       </c>
       <c r="F33">
-        <f>POWER(10, E33-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>2.8958835560872917E-4</v>
       </c>
       <c r="G33">
@@ -1820,7 +1831,7 @@
         <v>14.495410829669799</v>
       </c>
       <c r="I33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4928160325353274E-4</v>
       </c>
       <c r="J33">
@@ -1830,7 +1841,7 @@
         <v>14.517866326039499</v>
       </c>
       <c r="L33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5720334653301351E-4</v>
       </c>
     </row>
@@ -1842,7 +1853,7 @@
         <v>14.6771242067115</v>
       </c>
       <c r="C34">
-        <f>POWER(10, B34-10)/$N$3</f>
+        <f t="shared" si="0"/>
         <v>2.2684001519324647E-4</v>
       </c>
       <c r="D34">
@@ -1852,7 +1863,7 @@
         <v>14.9180955979009</v>
       </c>
       <c r="F34">
-        <f>POWER(10, E34-10)/$N$3</f>
+        <f t="shared" si="1"/>
         <v>3.9508547081907003E-4</v>
       </c>
       <c r="G34">
@@ -1862,7 +1873,7 @@
         <v>14.562215098334301</v>
       </c>
       <c r="I34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7410472572152997E-4</v>
       </c>
       <c r="J34">
@@ -1872,7 +1883,7 @@
         <v>14.5897747461592</v>
       </c>
       <c r="L34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8551123094169336E-4</v>
       </c>
     </row>
@@ -1884,7 +1895,7 @@
         <v>14.7393234623399</v>
       </c>
       <c r="C35">
-        <f>POWER(10, B35-10)/$N$3</f>
+        <f t="shared" ref="C35:C66" si="4">POWER(10, B35-10)/$N$3</f>
         <v>2.6176942759085267E-4</v>
       </c>
       <c r="D35">
@@ -1894,7 +1905,7 @@
         <v>15.0572400734886</v>
       </c>
       <c r="F35">
-        <f>POWER(10, E35-10)/$N$3</f>
+        <f t="shared" ref="F35:F66" si="5">POWER(10, E35-10)/$N$3</f>
         <v>5.4429649098266001E-4</v>
       </c>
       <c r="G35">
@@ -1904,7 +1915,7 @@
         <v>14.629713024788</v>
       </c>
       <c r="I35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0338011369399996E-4</v>
       </c>
       <c r="J35">
@@ -1914,7 +1925,7 @@
         <v>14.661266080433901</v>
       </c>
       <c r="L35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.1870642490360497E-4</v>
       </c>
     </row>
@@ -1926,7 +1937,7 @@
         <v>14.802566974810301</v>
       </c>
       <c r="C36">
-        <f>POWER(10, B36-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.0280457728310413E-4</v>
       </c>
       <c r="D36">
@@ -1936,7 +1947,7 @@
         <v>15.1954783459481</v>
       </c>
       <c r="F36">
-        <f>POWER(10, E36-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>7.4829666029612016E-4</v>
       </c>
       <c r="G36">
@@ -1946,7 +1957,7 @@
         <v>14.6975238136769</v>
       </c>
       <c r="I36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3774931518579195E-4</v>
       </c>
       <c r="J36">
@@ -1956,7 +1967,7 @@
         <v>14.733496246346</v>
       </c>
       <c r="L36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5828055284620377E-4</v>
       </c>
     </row>
@@ -1968,7 +1979,7 @@
         <v>14.868117870608501</v>
       </c>
       <c r="C37">
-        <f>POWER(10, B37-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.5213835539414602E-4</v>
       </c>
       <c r="D37">
@@ -1978,7 +1989,7 @@
         <v>15.3349857633425</v>
       </c>
       <c r="F37">
-        <f>POWER(10, E37-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.0317660284054682E-3</v>
       </c>
       <c r="G37">
@@ -1988,7 +1999,7 @@
         <v>14.7656489151624</v>
       </c>
       <c r="I37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7812778439112364E-4</v>
       </c>
       <c r="J37">
@@ -1998,7 +2009,7 @@
         <v>14.7877431236732</v>
       </c>
       <c r="L37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.9264329944102421E-4</v>
       </c>
     </row>
@@ -2010,7 +2021,7 @@
         <v>15.0081114038768</v>
       </c>
       <c r="C38">
-        <f>POWER(10, B38-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>4.8607900688169556E-4</v>
       </c>
       <c r="D38">
@@ -2020,7 +2031,7 @@
         <v>15.483638635761899</v>
       </c>
       <c r="F38">
-        <f>POWER(10, E38-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.4528945569562887E-3</v>
       </c>
       <c r="G38">
@@ -2030,7 +2041,7 @@
         <v>14.834480966111901</v>
       </c>
       <c r="I38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2589404675998913E-4</v>
       </c>
       <c r="J38">
@@ -2040,7 +2051,7 @@
         <v>14.831234900160901</v>
       </c>
       <c r="L38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2346728337892549E-4</v>
       </c>
     </row>
@@ -2052,7 +2063,7 @@
         <v>15.157055652880301</v>
       </c>
       <c r="C39">
-        <f>POWER(10, B39-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>6.8493776747319962E-4</v>
       </c>
       <c r="D39">
@@ -2062,7 +2073,7 @@
         <v>15.6280580600794</v>
       </c>
       <c r="F39">
-        <f>POWER(10, E39-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.0260656850044872E-3</v>
       </c>
       <c r="G39">
@@ -2072,7 +2083,7 @@
         <v>14.9032408833683</v>
       </c>
       <c r="I39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8180036949831092E-4</v>
       </c>
       <c r="J39">
@@ -2082,7 +2093,7 @@
         <v>14.8752468439405</v>
       </c>
       <c r="L39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5796643362891612E-4</v>
       </c>
     </row>
@@ -2094,7 +2105,7 @@
         <v>15.300478548628501</v>
       </c>
       <c r="C40">
-        <f>POWER(10, B40-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>9.5295854713663066E-4</v>
       </c>
       <c r="D40">
@@ -2104,7 +2115,7 @@
         <v>15.770774470942101</v>
       </c>
       <c r="F40">
-        <f>POWER(10, E40-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.8142970272283341E-3</v>
       </c>
       <c r="G40">
@@ -2114,7 +2125,7 @@
         <v>14.971924697828101</v>
       </c>
       <c r="I40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.4721891004391852E-4</v>
       </c>
       <c r="J40">
@@ -2124,7 +2135,7 @@
         <v>14.918995974928601</v>
       </c>
       <c r="L40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.9590540958461058E-4</v>
       </c>
     </row>
@@ -2136,7 +2147,7 @@
         <v>15.439455190953799</v>
       </c>
       <c r="C41">
-        <f>POWER(10, B41-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.3123529503590943E-3</v>
       </c>
       <c r="D41">
@@ -2146,7 +2157,7 @@
         <v>15.901584187607201</v>
       </c>
       <c r="F41">
-        <f>POWER(10, E41-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.8034669654698557E-3</v>
       </c>
       <c r="G41">
@@ -2156,7 +2167,7 @@
         <v>15.041321686219</v>
       </c>
       <c r="I41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.2470734934121916E-4</v>
       </c>
       <c r="J41">
@@ -2166,7 +2177,7 @@
         <v>14.963268351201799</v>
       </c>
       <c r="L41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3839320311694354E-4</v>
       </c>
     </row>
@@ -2178,7 +2189,7 @@
         <v>15.592448258200999</v>
       </c>
       <c r="C42">
-        <f>POWER(10, B42-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.8665675834324362E-3</v>
       </c>
       <c r="D42">
@@ -2188,7 +2199,7 @@
         <v>16.422895846885002</v>
       </c>
       <c r="F42">
-        <f>POWER(10, E42-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.2632558203024141E-2</v>
       </c>
       <c r="G42">
@@ -2198,7 +2209,7 @@
         <v>15.1038694372879</v>
       </c>
       <c r="I42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0598921965031066E-4</v>
       </c>
       <c r="J42">
@@ -2208,7 +2219,7 @@
         <v>15.007672106510499</v>
       </c>
       <c r="L42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.8558757704246042E-4</v>
       </c>
     </row>
@@ -2220,7 +2231,7 @@
         <v>15.745553223326899</v>
       </c>
       <c r="C43">
-        <f>POWER(10, B43-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.6555145437939898E-3</v>
       </c>
       <c r="D43">
@@ -2230,7 +2241,7 @@
         <v>16.318440571332498</v>
       </c>
       <c r="F43">
-        <f>POWER(10, E43-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>9.9319844818487896E-3</v>
       </c>
       <c r="G43">
@@ -2240,7 +2251,7 @@
         <v>15.147092629628199</v>
       </c>
       <c r="I43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.6940367242704899E-4</v>
       </c>
       <c r="J43">
@@ -2250,7 +2261,7 @@
         <v>15.0526045625497</v>
       </c>
       <c r="L43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.3851775118703919E-4</v>
       </c>
     </row>
@@ -2262,7 +2273,7 @@
         <v>15.8924225799748</v>
       </c>
       <c r="C44">
-        <f>POWER(10, B44-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.7240717604682836E-3</v>
       </c>
       <c r="D44">
@@ -2272,7 +2283,7 @@
         <v>16.214649667319001</v>
       </c>
       <c r="F44">
-        <f>POWER(10, E44-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>7.8206910235430419E-3</v>
       </c>
       <c r="G44">
@@ -2282,7 +2293,7 @@
         <v>15.1892378472988</v>
       </c>
       <c r="I44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.3762106071058222E-4</v>
       </c>
       <c r="J44">
@@ -2292,7 +2303,7 @@
         <v>15.0972734245968</v>
       </c>
       <c r="L44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.968550675874121E-4</v>
       </c>
     </row>
@@ -2304,7 +2315,7 @@
         <v>16.028037371805599</v>
       </c>
       <c r="C45">
-        <f>POWER(10, B45-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>5.0890044753188418E-3</v>
       </c>
       <c r="D45">
@@ -2314,7 +2325,7 @@
         <v>16.116193053934399</v>
       </c>
       <c r="F45">
-        <f>POWER(10, E45-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>6.2343117402355232E-3</v>
       </c>
       <c r="G45">
@@ -2324,7 +2335,7 @@
         <v>15.2315003296759</v>
       </c>
       <c r="I45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1300981884360973E-4</v>
       </c>
       <c r="J45">
@@ -2334,7 +2345,7 @@
         <v>15.1420748422576</v>
       </c>
       <c r="L45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.6171396962183245E-4</v>
       </c>
     </row>
@@ -2346,7 +2357,7 @@
         <v>16.193293613335701</v>
       </c>
       <c r="C46">
-        <f>POWER(10, B46-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>7.4454178188106367E-3</v>
       </c>
       <c r="D46">
@@ -2356,7 +2367,7 @@
         <v>16.013688513809299</v>
       </c>
       <c r="F46">
-        <f>POWER(10, E46-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>4.9236137380389289E-3</v>
       </c>
       <c r="G46">
@@ -2366,7 +2377,7 @@
         <v>15.2730748800759</v>
       </c>
       <c r="I46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.9468538091711988E-4</v>
       </c>
       <c r="J46">
@@ -2376,7 +2387,7 @@
         <v>15.187009208893301</v>
       </c>
       <c r="L46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.3384555818926196E-4</v>
       </c>
     </row>
@@ -2388,7 +2399,7 @@
         <v>16.350592407533501</v>
       </c>
       <c r="C47">
-        <f>POWER(10, B47-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.0695174345101881E-2</v>
       </c>
       <c r="D47">
@@ -2398,7 +2409,7 @@
         <v>15.819806217283199</v>
       </c>
       <c r="F47">
-        <f>POWER(10, E47-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.1506610082628365E-3</v>
       </c>
       <c r="G47">
@@ -2408,7 +2419,7 @@
         <v>15.315570630320501</v>
       </c>
       <c r="I47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.8665674987890618E-4</v>
       </c>
       <c r="J47">
@@ -2418,7 +2429,7 @@
         <v>15.232076919032099</v>
       </c>
       <c r="L47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.1408992496404616E-4</v>
       </c>
     </row>
@@ -2430,7 +2441,7 @@
         <v>16.489680931441001</v>
       </c>
       <c r="C48">
-        <f>POWER(10, B48-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.4732498055012927E-2</v>
       </c>
       <c r="D48">
@@ -2440,7 +2451,7 @@
         <v>15.719186799549499</v>
       </c>
       <c r="F48">
-        <f>POWER(10, E48-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.4990920936558162E-3</v>
       </c>
       <c r="G48">
@@ -2450,7 +2461,7 @@
         <v>15.357779630729301</v>
       </c>
       <c r="I48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0873643536775141E-3</v>
       </c>
       <c r="J48">
@@ -2460,7 +2471,7 @@
         <v>15.277278368373301</v>
       </c>
       <c r="L48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.0338698484964265E-4</v>
       </c>
     </row>
@@ -2472,7 +2483,7 @@
         <v>16.6241547750191</v>
       </c>
       <c r="C49">
-        <f>POWER(10, B49-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.0079377098077767E-2</v>
       </c>
       <c r="D49">
@@ -2482,7 +2493,7 @@
         <v>15.0388735727584</v>
       </c>
       <c r="F49">
-        <f>POWER(10, E49-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>5.2175790030750777E-4</v>
       </c>
       <c r="G49">
@@ -2492,7 +2503,7 @@
         <v>15.4005110631765</v>
       </c>
       <c r="I49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.199793553574433E-3</v>
       </c>
       <c r="J49">
@@ -2502,7 +2513,7 @@
         <v>15.322613953790199</v>
       </c>
       <c r="L49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0027886615483082E-3</v>
       </c>
     </row>
@@ -2514,7 +2525,7 @@
         <v>15.886091580888699</v>
       </c>
       <c r="C50">
-        <f>POWER(10, B50-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>3.6701772754531552E-3</v>
       </c>
       <c r="D50">
@@ -2524,7 +2535,7 @@
         <v>15.6237386752176</v>
       </c>
       <c r="F50">
-        <f>POWER(10, E50-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.006014815561051E-3</v>
       </c>
       <c r="G50">
@@ -2534,7 +2545,7 @@
         <v>15.442954155468099</v>
       </c>
       <c r="I50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3229688434311286E-3</v>
       </c>
       <c r="J50">
@@ -2544,7 +2555,7 @@
         <v>15.3676788224258</v>
       </c>
       <c r="L50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1124340753426673E-3</v>
       </c>
     </row>
@@ -2556,7 +2567,7 @@
         <v>15.7476481575384</v>
       </c>
       <c r="C51">
-        <f>POWER(10, B51-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.6683550649369797E-3</v>
       </c>
       <c r="D51">
@@ -2566,7 +2577,7 @@
         <v>15.524366314600099</v>
       </c>
       <c r="F51">
-        <f>POWER(10, E51-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.5957386921863226E-3</v>
       </c>
       <c r="G51">
@@ -2576,7 +2587,7 @@
         <v>15.4859225772156</v>
       </c>
       <c r="I51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4605554116272899E-3</v>
       </c>
       <c r="J51">
@@ -2586,7 +2597,7 @@
         <v>15.412876229960601</v>
       </c>
       <c r="L51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.2344448465027751E-3</v>
       </c>
     </row>
@@ -2598,7 +2609,7 @@
         <v>16.046201856716301</v>
       </c>
       <c r="C52">
-        <f>POWER(10, B52-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>5.3063674186165193E-3</v>
       </c>
       <c r="D52">
@@ -2608,7 +2619,7 @@
         <v>14.911994971840301</v>
       </c>
       <c r="F52">
-        <f>POWER(10, E52-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.8957442006258319E-4</v>
       </c>
       <c r="G52">
@@ -2618,7 +2629,7 @@
         <v>15.528601059667899</v>
       </c>
       <c r="I52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.611374626172732E-3</v>
       </c>
       <c r="J52">
@@ -2628,7 +2639,7 @@
         <v>15.4586142043559</v>
       </c>
       <c r="L52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3715437496906581E-3</v>
       </c>
     </row>
@@ -2640,7 +2651,7 @@
         <v>15.6491898570051</v>
       </c>
       <c r="C53">
-        <f>POWER(10, B53-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>2.1270873166332254E-3</v>
       </c>
       <c r="D53">
@@ -2650,7 +2661,7 @@
         <v>15.4301011553991</v>
       </c>
       <c r="F53">
-        <f>POWER(10, E53-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.2843891151728931E-3</v>
       </c>
       <c r="G53">
@@ -2660,7 +2671,7 @@
         <v>15.5718077850628</v>
       </c>
       <c r="I53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.779931324111343E-3</v>
       </c>
       <c r="J53">
@@ -2670,7 +2681,7 @@
         <v>15.5044879069742</v>
       </c>
       <c r="L53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5243453418392751E-3</v>
       </c>
     </row>
@@ -2682,7 +2693,7 @@
         <v>15.5513471428023</v>
       </c>
       <c r="C54">
-        <f>POWER(10, B54-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.6980192280036249E-3</v>
       </c>
       <c r="D54">
@@ -2692,7 +2703,7 @@
         <v>14.7801052199758</v>
       </c>
       <c r="F54">
-        <f>POWER(10, E54-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.875415973273757E-4</v>
       </c>
       <c r="G54">
@@ -2702,7 +2713,7 @@
         <v>15.614722963153801</v>
       </c>
       <c r="I54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9648003378760904E-3</v>
       </c>
       <c r="J54">
@@ -2712,7 +2723,7 @@
         <v>15.5509078124963</v>
       </c>
       <c r="L54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6963023880606641E-3</v>
       </c>
     </row>
@@ -2724,7 +2735,7 @@
         <v>16.148935841278501</v>
       </c>
       <c r="C55">
-        <f>POWER(10, B55-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>6.7225076060410749E-3</v>
       </c>
       <c r="D55">
@@ -2734,7 +2745,7 @@
         <v>15.336408381573399</v>
       </c>
       <c r="F55">
-        <f>POWER(10, E55-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>1.0351513254822707E-3</v>
       </c>
       <c r="G55">
@@ -2744,7 +2755,7 @@
         <v>15.658169313832399</v>
       </c>
       <c r="I55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.1715247060779723E-3</v>
       </c>
       <c r="J55">
@@ -2754,7 +2765,7 @@
         <v>15.5970553979787</v>
       </c>
       <c r="L55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8864741519414967E-3</v>
       </c>
     </row>
@@ -2766,7 +2777,7 @@
         <v>15.454676523047301</v>
       </c>
       <c r="C56">
-        <f>POWER(10, B56-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.3591643790747197E-3</v>
       </c>
       <c r="D56">
@@ -2776,7 +2787,7 @@
         <v>14.702644813377001</v>
       </c>
       <c r="F56">
-        <f>POWER(10, E56-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.4056933870013713E-4</v>
       </c>
       <c r="G56">
@@ -2786,7 +2797,7 @@
         <v>15.7009084619937</v>
       </c>
       <c r="I56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.3960943935805975E-3</v>
       </c>
       <c r="J56">
@@ -2796,7 +2807,7 @@
         <v>15.643339927212001</v>
       </c>
       <c r="L56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.0986276388295783E-3</v>
       </c>
     </row>
@@ -2808,7 +2819,7 @@
         <v>15.3586068292853</v>
       </c>
       <c r="C57">
-        <f>POWER(10, B57-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.0894374248522046E-3</v>
       </c>
       <c r="D57">
@@ -2818,7 +2829,7 @@
         <v>15.2388635406136</v>
       </c>
       <c r="F57">
-        <f>POWER(10, E57-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>8.2691144254515303E-4</v>
       </c>
       <c r="G57">
@@ -2828,7 +2839,7 @@
         <v>15.7450098052089</v>
       </c>
       <c r="I57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.6521938654771753E-3</v>
       </c>
       <c r="J57">
@@ -2838,7 +2849,7 @@
         <v>15.689348073143799</v>
       </c>
       <c r="L57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.3331546917117162E-3</v>
       </c>
     </row>
@@ -2850,7 +2861,7 @@
         <v>15.2625809140601</v>
       </c>
       <c r="C58">
-        <f>POWER(10, B58-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>8.7332597026559627E-4</v>
       </c>
       <c r="D58">
@@ -2860,7 +2871,7 @@
         <v>14.7112246582181</v>
       </c>
       <c r="F58">
-        <f>POWER(10, E58-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.4536924082936459E-4</v>
       </c>
       <c r="G58">
@@ -2870,7 +2881,7 @@
         <v>15.7879859854621</v>
       </c>
       <c r="I58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.9280699424703324E-3</v>
       </c>
       <c r="J58">
@@ -2880,7 +2891,7 @@
         <v>15.7359064824726</v>
       </c>
       <c r="L58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5971793637258305E-3</v>
       </c>
     </row>
@@ -2892,7 +2903,7 @@
         <v>15.171475566623799</v>
       </c>
       <c r="C59">
-        <f>POWER(10, B59-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>7.080615763510003E-4</v>
       </c>
       <c r="D59">
@@ -2902,7 +2913,7 @@
         <v>14.765681510414201</v>
       </c>
       <c r="F59">
-        <f>POWER(10, E59-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.7814865959390595E-4</v>
       </c>
       <c r="G59">
@@ -2912,7 +2923,7 @@
         <v>15.8323319155277</v>
       </c>
       <c r="I59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2428538524660608E-3</v>
       </c>
       <c r="J59">
@@ -2922,7 +2933,7 @@
         <v>15.784684127437901</v>
       </c>
       <c r="L59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.9058927968932369E-3</v>
       </c>
     </row>
@@ -2934,7 +2945,7 @@
         <v>15.2036623114639</v>
       </c>
       <c r="C60">
-        <f>POWER(10, B60-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>7.6253147095987699E-4</v>
       </c>
       <c r="D60">
@@ -2944,7 +2955,7 @@
         <v>14.753614960837099</v>
       </c>
       <c r="F60">
-        <f>POWER(10, E60-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.7052687876677744E-4</v>
       </c>
       <c r="G60">
@@ -2954,7 +2965,7 @@
         <v>15.8734533902955</v>
       </c>
       <c r="I60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.5649123081728856E-3</v>
       </c>
       <c r="J60">
@@ -2964,7 +2975,7 @@
         <v>15.8357007705992</v>
       </c>
       <c r="L60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2681067321516954E-3</v>
       </c>
     </row>
@@ -2976,7 +2987,7 @@
         <v>15.245160877682</v>
       </c>
       <c r="C61">
-        <f>POWER(10, B61-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>8.3898913880173025E-4</v>
       </c>
       <c r="D61">
@@ -2986,7 +2997,7 @@
         <v>14.7871324668579</v>
       </c>
       <c r="F61">
-        <f>POWER(10, E61-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>2.9223210598995999E-4</v>
       </c>
       <c r="G61">
@@ -2996,7 +3007,7 @@
         <v>15.909226894981099</v>
       </c>
       <c r="I61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8709927325660874E-3</v>
       </c>
       <c r="J61">
@@ -3006,7 +3017,7 @@
         <v>15.885625540152599</v>
       </c>
       <c r="L61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.6662409263243227E-3</v>
       </c>
     </row>
@@ -3018,7 +3029,7 @@
         <v>15.287982098751201</v>
       </c>
       <c r="C62">
-        <f>POWER(10, B62-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>9.2592873002832633E-4</v>
       </c>
       <c r="D62">
@@ -3028,7 +3039,7 @@
         <v>14.8224119696843</v>
       </c>
       <c r="F62">
-        <f>POWER(10, E62-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.1696216940496586E-4</v>
       </c>
       <c r="G62">
@@ -3038,7 +3049,7 @@
         <v>15.943819656219301</v>
       </c>
       <c r="I62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.1919405726288574E-3</v>
       </c>
       <c r="J62">
@@ -3048,7 +3059,7 @@
         <v>15.9348672793249</v>
       </c>
       <c r="L62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.1064140796118727E-3</v>
       </c>
     </row>
@@ -3060,7 +3071,7 @@
         <v>15.33011506645</v>
       </c>
       <c r="C63">
-        <f>POWER(10, B63-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.0202592183400938E-3</v>
       </c>
       <c r="D63">
@@ -3070,7 +3081,7 @@
         <v>14.862477980242801</v>
       </c>
       <c r="F63">
-        <f>POWER(10, E63-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.4759493640716975E-4</v>
       </c>
       <c r="G63">
@@ -3080,7 +3091,7 @@
         <v>15.9780662883558</v>
       </c>
       <c r="I63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.5358820145446413E-3</v>
       </c>
       <c r="J63">
@@ -3090,7 +3101,7 @@
         <v>15.985947764739601</v>
       </c>
       <c r="L63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6189496243889154E-3</v>
       </c>
     </row>
@@ -3102,7 +3113,7 @@
         <v>15.3723641506484</v>
       </c>
       <c r="C64">
-        <f>POWER(10, B64-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.1245003932235326E-3</v>
       </c>
       <c r="D64">
@@ -3112,7 +3123,7 @@
         <v>14.9038312871063</v>
       </c>
       <c r="F64">
-        <f>POWER(10, E64-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>3.8231976282671466E-4</v>
       </c>
       <c r="G64">
@@ -3122,7 +3133,7 @@
         <v>16.015342479089501</v>
       </c>
       <c r="I64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.9424005590306807E-3</v>
       </c>
       <c r="J64">
@@ -3132,7 +3143,7 @@
         <v>16.035500479441598</v>
       </c>
       <c r="L64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1772118962899053E-3</v>
       </c>
     </row>
@@ -3144,7 +3155,7 @@
         <v>15.4139167202051</v>
       </c>
       <c r="C65">
-        <f>POWER(10, B65-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.237405896505595E-3</v>
       </c>
       <c r="D65">
@@ -3154,7 +3165,7 @@
         <v>14.944905553032999</v>
       </c>
       <c r="F65">
-        <f>POWER(10, E65-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>4.2024350889244608E-4</v>
       </c>
       <c r="G65">
@@ -3164,7 +3175,7 @@
         <v>16.056939289032901</v>
       </c>
       <c r="I65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.439196516481757E-3</v>
       </c>
       <c r="J65">
@@ -3174,7 +3185,7 @@
         <v>16.086479346667399</v>
       </c>
       <c r="L65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.8220349426721194E-3</v>
       </c>
     </row>
@@ -3186,7 +3197,7 @@
         <v>15.4572119494725</v>
       </c>
       <c r="C66">
-        <f>POWER(10, B66-10)/$N$3</f>
+        <f t="shared" si="4"/>
         <v>1.3671224355180185E-3</v>
       </c>
       <c r="D66">
@@ -3196,7 +3207,7 @@
         <v>14.9837221063926</v>
       </c>
       <c r="F66">
-        <f>POWER(10, E66-10)/$N$3</f>
+        <f t="shared" si="5"/>
         <v>4.5953391312193178E-4</v>
       </c>
       <c r="G66">
@@ -3206,7 +3217,7 @@
         <v>16.1007668842987</v>
       </c>
       <c r="I66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.0167552458473914E-3</v>
       </c>
       <c r="J66">
@@ -3216,7 +3227,7 @@
         <v>16.137620282105999</v>
       </c>
       <c r="L66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.549614563975791E-3</v>
       </c>
     </row>
@@ -3228,7 +3239,7 @@
         <v>15.499402582261601</v>
       </c>
       <c r="C67">
-        <f>POWER(10, B67-10)/$N$3</f>
+        <f t="shared" ref="C67:C98" si="6">POWER(10, B67-10)/$N$3</f>
         <v>1.5066002780657472E-3</v>
       </c>
       <c r="D67">
@@ -3238,7 +3249,7 @@
         <v>15.022243336719299</v>
       </c>
       <c r="F67">
-        <f>POWER(10, E67-10)/$N$3</f>
+        <f t="shared" ref="F67:F98" si="7">POWER(10, E67-10)/$N$3</f>
         <v>5.0215616360133281E-4</v>
       </c>
       <c r="G67">
@@ -3248,7 +3259,7 @@
         <v>16.144288377110101</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I116" si="2">POWER(10, H67-10)/$N$3</f>
+        <f t="shared" ref="I67:I116" si="8">POWER(10, H67-10)/$N$3</f>
         <v>6.6509523761772221E-3</v>
       </c>
       <c r="J67">
@@ -3258,7 +3269,7 @@
         <v>16.187643146284898</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L115" si="3">POWER(10, K67-10)/$N$3</f>
+        <f t="shared" ref="L67:L115" si="9">POWER(10, K67-10)/$N$3</f>
         <v>7.3491753091174897E-3</v>
       </c>
     </row>
@@ -3270,7 +3281,7 @@
         <v>15.5429379276568</v>
       </c>
       <c r="C68">
-        <f>POWER(10, B68-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.6654568635227928E-3</v>
       </c>
       <c r="D68">
@@ -3280,7 +3291,7 @@
         <v>15.0604664505816</v>
       </c>
       <c r="F68">
-        <f>POWER(10, E68-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>5.4835513102685759E-4</v>
       </c>
       <c r="G68">
@@ -3290,7 +3301,7 @@
         <v>16.183533039270401</v>
       </c>
       <c r="I68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.279951739129634E-3</v>
       </c>
       <c r="J68">
@@ -3300,7 +3311,7 @@
         <v>16.2391056941307</v>
       </c>
       <c r="L68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.2737263963041912E-3</v>
       </c>
     </row>
@@ -3312,7 +3323,7 @@
         <v>15.5853625504615</v>
       </c>
       <c r="C69">
-        <f>POWER(10, B69-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.8363607913557145E-3</v>
       </c>
       <c r="D69">
@@ -3322,7 +3333,7 @@
         <v>15.0983886710174</v>
       </c>
       <c r="F69">
-        <f>POWER(10, E69-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>5.9838973105477223E-4</v>
       </c>
       <c r="G69">
@@ -3332,7 +3343,7 @@
         <v>16.185472159524899</v>
       </c>
       <c r="I69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.3125293215731395E-3</v>
       </c>
       <c r="J69">
@@ -3342,7 +3353,7 @@
         <v>16.290302267068999</v>
       </c>
       <c r="L69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.3088863483356925E-3</v>
       </c>
     </row>
@@ -3354,7 +3365,7 @@
         <v>15.629551489383701</v>
       </c>
       <c r="C70">
-        <f>POWER(10, B70-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.0330448072793422E-3</v>
       </c>
       <c r="D70">
@@ -3364,7 +3375,7 @@
         <v>15.1332135410116</v>
       </c>
       <c r="F70">
-        <f>POWER(10, E70-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>6.4834923388527865E-4</v>
       </c>
       <c r="G70">
@@ -3374,7 +3385,7 @@
         <v>16.225108964281901</v>
       </c>
       <c r="I70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.0113263817750829E-3</v>
       </c>
       <c r="J70">
@@ -3384,7 +3395,7 @@
         <v>16.340367508800501</v>
       </c>
       <c r="L70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.0446311447324682E-2</v>
       </c>
     </row>
@@ -3396,7 +3407,7 @@
         <v>15.672625806438401</v>
       </c>
       <c r="C71">
-        <f>POWER(10, B71-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.2450254439194055E-3</v>
       </c>
       <c r="D71">
@@ -3406,7 +3417,7 @@
         <v>15.169318732541401</v>
       </c>
       <c r="F71">
-        <f>POWER(10, E71-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>7.0455385179363738E-4</v>
       </c>
       <c r="G71">
@@ -3416,7 +3427,7 @@
         <v>16.268108559979801</v>
       </c>
       <c r="I71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.8451259408900296E-3</v>
       </c>
       <c r="J71">
@@ -3426,7 +3437,7 @@
         <v>16.381512517204001</v>
       </c>
       <c r="L71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1484391212522852E-2</v>
       </c>
     </row>
@@ -3438,7 +3449,7 @@
         <v>15.7162332657861</v>
       </c>
       <c r="C72">
-        <f>POWER(10, B72-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.4821540222590638E-3</v>
       </c>
       <c r="D72">
@@ -3448,7 +3459,7 @@
         <v>15.2051091008322</v>
       </c>
       <c r="F72">
-        <f>POWER(10, E72-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>7.6507597043345467E-4</v>
       </c>
       <c r="G72">
@@ -3458,7 +3469,7 @@
         <v>16.308641556098902</v>
       </c>
       <c r="I72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.7103976957479306E-3</v>
       </c>
       <c r="J72">
@@ -3468,7 +3479,7 @@
         <v>16.417565133879801</v>
       </c>
       <c r="L72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.2478448611971298E-2</v>
       </c>
     </row>
@@ -3480,7 +3491,7 @@
         <v>15.759130900153201</v>
       </c>
       <c r="C73">
-        <f>POWER(10, B73-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.7398473138639939E-3</v>
       </c>
       <c r="D73">
@@ -3490,7 +3501,7 @@
         <v>15.240582013307399</v>
       </c>
       <c r="F73">
-        <f>POWER(10, E73-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>8.3018995505880499E-4</v>
       </c>
       <c r="G73">
@@ -3500,7 +3511,7 @@
         <v>16.345395830721898</v>
       </c>
       <c r="I73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.0567963185725783E-2</v>
       </c>
       <c r="J73">
@@ -3510,7 +3521,7 @@
         <v>16.454564886158099</v>
       </c>
       <c r="L73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.3588150461003069E-2</v>
       </c>
     </row>
@@ -3522,7 +3533,7 @@
         <v>15.803812521806799</v>
       </c>
       <c r="C74">
-        <f>POWER(10, B74-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.0367426065317652E-3</v>
       </c>
       <c r="D74">
@@ -3532,7 +3543,7 @@
         <v>15.2761376826711</v>
       </c>
       <c r="F74">
-        <f>POWER(10, E74-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>9.010173288855806E-4</v>
       </c>
       <c r="G74">
@@ -3542,7 +3553,7 @@
         <v>16.380936990518698</v>
       </c>
       <c r="I74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.1469182186583734E-2</v>
       </c>
       <c r="J74">
@@ -3552,7 +3563,7 @@
         <v>16.490778277307701</v>
       </c>
       <c r="L74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.4769770201280319E-2</v>
       </c>
     </row>
@@ -3564,7 +3575,7 @@
         <v>15.8473670941629</v>
       </c>
       <c r="C75">
-        <f>POWER(10, B75-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.3570866821204365E-3</v>
       </c>
       <c r="D75">
@@ -3574,7 +3585,7 @@
         <v>15.3117763019919</v>
       </c>
       <c r="F75">
-        <f>POWER(10, E75-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>9.7807410970044231E-4</v>
       </c>
       <c r="G75">
@@ -3584,7 +3595,7 @@
         <v>16.4169883405688</v>
       </c>
       <c r="I75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.2461886789154731E-2</v>
       </c>
       <c r="J75">
@@ -3594,7 +3605,7 @@
         <v>16.527943027753999</v>
       </c>
       <c r="L75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.6089349611942163E-2</v>
       </c>
     </row>
@@ -3606,7 +3617,7 @@
         <v>15.8914607530597</v>
       </c>
       <c r="C76">
-        <f>POWER(10, B76-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.7158332285072639E-3</v>
       </c>
       <c r="D76">
@@ -3616,7 +3627,7 @@
         <v>15.3462839726176</v>
       </c>
       <c r="F76">
-        <f>POWER(10, E76-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.0589597019291606E-3</v>
       </c>
       <c r="G76">
@@ -3626,7 +3637,7 @@
         <v>16.452685169941201</v>
       </c>
       <c r="I76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.3529465231820763E-2</v>
       </c>
       <c r="J76">
@@ -3636,7 +3647,7 @@
         <v>16.564317910341501</v>
       </c>
       <c r="L76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.7494976817259793E-2</v>
       </c>
     </row>
@@ -3648,7 +3659,7 @@
         <v>15.935256879865101</v>
       </c>
       <c r="C77">
-        <f>POWER(10, B77-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>4.1100995488809319E-3</v>
       </c>
       <c r="D77">
@@ -3658,7 +3669,7 @@
         <v>15.3731650677034</v>
       </c>
       <c r="F77">
-        <f>POWER(10, E77-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.1265760873775839E-3</v>
       </c>
       <c r="G77">
@@ -3668,7 +3679,7 @@
         <v>16.4893292419343</v>
       </c>
       <c r="I77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.4720572580768728E-2</v>
       </c>
       <c r="J77">
@@ -3678,7 +3689,7 @@
         <v>16.6020861858599</v>
       </c>
       <c r="L77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.9084537818649685E-2</v>
       </c>
     </row>
@@ -3690,7 +3701,7 @@
         <v>15.9795950829949</v>
       </c>
       <c r="C78">
-        <f>POWER(10, B78-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>4.5518772711153699E-3</v>
       </c>
       <c r="D78">
@@ -3700,7 +3711,7 @@
         <v>15.400093248668499</v>
       </c>
       <c r="F78">
-        <f>POWER(10, E78-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.1986398430921842E-3</v>
       </c>
       <c r="G78">
@@ -3710,7 +3721,7 @@
         <v>16.5260549290558</v>
       </c>
       <c r="I78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.6019552868014743E-2</v>
       </c>
       <c r="J78">
@@ -3720,7 +3731,7 @@
         <v>16.6386242435422</v>
       </c>
       <c r="L78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.075963457650885E-2</v>
       </c>
     </row>
@@ -3732,7 +3743,7 @@
         <v>16.022789039999001</v>
       </c>
       <c r="C79">
-        <f>POWER(10, B79-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>5.0278753358433629E-3</v>
       </c>
       <c r="D79">
@@ -3742,7 +3753,7 @@
         <v>15.4266617916811</v>
       </c>
       <c r="F79">
-        <f>POWER(10, E79-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.2742576591488835E-3</v>
       </c>
       <c r="G79">
@@ -3752,7 +3763,7 @@
         <v>16.562862413082101</v>
       </c>
       <c r="I79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.7436442183327548E-2</v>
       </c>
       <c r="J79">
@@ -3762,7 +3773,7 @@
         <v>16.675682446403801</v>
       </c>
       <c r="L79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.2608820581187156E-2</v>
       </c>
     </row>
@@ -3774,7 +3785,7 @@
         <v>16.0652524497788</v>
       </c>
       <c r="C80">
-        <f>POWER(10, B80-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>5.5443151792862345E-3</v>
       </c>
       <c r="D80">
@@ -3784,7 +3795,7 @@
         <v>15.4524611872242</v>
       </c>
       <c r="F80">
-        <f>POWER(10, E80-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.3522489354384371E-3</v>
       </c>
       <c r="G80">
@@ -3794,7 +3805,7 @@
         <v>16.598438722173601</v>
       </c>
       <c r="I80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.8924925701998118E-2</v>
       </c>
       <c r="J80">
@@ -3804,7 +3815,7 @@
         <v>16.712382475562698</v>
       </c>
       <c r="L80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.4602426133568108E-2</v>
       </c>
     </row>
@@ -3816,7 +3827,7 @@
         <v>16.1086779446034</v>
       </c>
       <c r="C81">
-        <f>POWER(10, B81-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>6.1273601194185316E-3</v>
       </c>
       <c r="D81">
@@ -3826,7 +3837,7 @@
         <v>15.4791200764318</v>
       </c>
       <c r="F81">
-        <f>POWER(10, E81-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.4378564747797114E-3</v>
       </c>
       <c r="G81">
@@ -3836,7 +3847,7 @@
         <v>16.634968752476802</v>
       </c>
       <c r="I81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.058563240970256E-2</v>
       </c>
       <c r="J81">
@@ -3846,7 +3857,7 @@
         <v>16.7500466484491</v>
       </c>
       <c r="L81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.6831324360996105E-2</v>
       </c>
     </row>
@@ -3858,7 +3869,7 @@
         <v>16.150943070310401</v>
       </c>
       <c r="C82">
-        <f>POWER(10, B82-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>6.7536497079732838E-3</v>
       </c>
       <c r="D82">
@@ -3868,7 +3879,7 @@
         <v>15.507051672031899</v>
       </c>
       <c r="F82">
-        <f>POWER(10, E82-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.5333706033353294E-3</v>
       </c>
       <c r="G82">
@@ -3878,7 +3889,7 @@
         <v>16.671579178480901</v>
       </c>
       <c r="I82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.2396215591628556E-2</v>
       </c>
       <c r="J82">
@@ -3888,7 +3899,7 @@
         <v>16.787353015703701</v>
       </c>
       <c r="L82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.9238054863523891E-2</v>
       </c>
     </row>
@@ -3900,7 +3911,7 @@
         <v>16.1941731469987</v>
       </c>
       <c r="C83">
-        <f>POWER(10, B83-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>7.4605115659540748E-3</v>
       </c>
       <c r="D83">
@@ -3910,7 +3921,7 @@
         <v>15.532575911510101</v>
       </c>
       <c r="F83">
-        <f>POWER(10, E83-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.6261903234809892E-3</v>
       </c>
       <c r="G83">
@@ -3920,7 +3931,7 @@
         <v>16.70959202025</v>
       </c>
       <c r="I83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.4444855886267849E-2</v>
       </c>
       <c r="J83">
@@ -3930,7 +3941,7 @@
         <v>16.824742473176901</v>
       </c>
       <c r="L83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.1866761806564718E-2</v>
       </c>
     </row>
@@ -3942,7 +3953,7 @@
         <v>16.237090756952199</v>
       </c>
       <c r="C84">
-        <f>POWER(10, B84-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>8.2354288213298075E-3</v>
       </c>
       <c r="D84">
@@ -3952,7 +3963,7 @@
         <v>15.5593730162119</v>
       </c>
       <c r="F84">
-        <f>POWER(10, E84-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.7296908069130276E-3</v>
       </c>
       <c r="G84">
@@ -3962,7 +3973,7 @@
         <v>16.745483498164798</v>
       </c>
       <c r="I84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.6550882401514167E-2</v>
       </c>
       <c r="J84">
@@ -3972,7 +3983,7 @@
         <v>16.8622152059305</v>
       </c>
       <c r="L84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.4738468415449961E-2</v>
       </c>
     </row>
@@ -3984,7 +3995,7 @@
         <v>16.280122106658101</v>
       </c>
       <c r="C85">
-        <f>POWER(10, B85-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>9.093217260876375E-3</v>
       </c>
       <c r="D85">
@@ -3994,7 +4005,7 @@
         <v>15.585805348825801</v>
       </c>
       <c r="F85">
-        <f>POWER(10, E85-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.838234064582204E-3</v>
       </c>
       <c r="G85">
@@ -4004,7 +4015,7 @@
         <v>16.782337146262002</v>
       </c>
       <c r="I85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.8902313485870811E-2</v>
       </c>
       <c r="J85">
@@ -4014,7 +4025,7 @@
         <v>16.8930880188279</v>
       </c>
       <c r="L85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.7297822671769808E-2</v>
       </c>
     </row>
@@ -4026,7 +4037,7 @@
         <v>16.324128409110902</v>
       </c>
       <c r="C86">
-        <f>POWER(10, B86-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.0062916525081563E-2</v>
       </c>
       <c r="D86">
@@ -4036,7 +4047,7 @@
         <v>15.6135177209521</v>
       </c>
       <c r="F86">
-        <f>POWER(10, E86-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>1.9593552366071782E-3</v>
       </c>
       <c r="G86">
@@ -4046,7 +4057,7 @@
         <v>16.816610968418999</v>
       </c>
       <c r="I86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.1275656123678532E-2</v>
       </c>
       <c r="J86">
@@ -4056,7 +4067,7 @@
         <v>16.923571076046201</v>
       </c>
       <c r="L86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.000981442627162E-2</v>
       </c>
     </row>
@@ -4068,7 +4079,7 @@
         <v>16.366527231853102</v>
       </c>
       <c r="C87">
-        <f>POWER(10, B87-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.109488213297165E-2</v>
       </c>
       <c r="D87">
@@ -4078,7 +4089,7 @@
         <v>15.642104309687999</v>
       </c>
       <c r="F87">
-        <f>POWER(10, E87-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.0926652887285546E-3</v>
       </c>
       <c r="G87">
@@ -4088,7 +4099,7 @@
         <v>16.850066090836901</v>
       </c>
       <c r="I87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.3780148297612514E-2</v>
       </c>
       <c r="J87">
@@ -4098,7 +4109,7 @@
         <v>16.953215003142802</v>
       </c>
       <c r="L87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.2836153300317398E-2</v>
       </c>
     </row>
@@ -4110,7 +4121,7 @@
         <v>16.410767093369401</v>
       </c>
       <c r="C88">
-        <f>POWER(10, B88-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.2284643403099784E-2</v>
       </c>
       <c r="D88">
@@ -4120,7 +4131,7 @@
         <v>15.670743237241499</v>
       </c>
       <c r="F88">
-        <f>POWER(10, E88-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.2353148239092086E-3</v>
       </c>
       <c r="G88">
@@ -4130,7 +4141,7 @@
         <v>16.8813618155793</v>
       </c>
       <c r="I88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6304233896528773E-2</v>
       </c>
       <c r="J88">
@@ -4140,7 +4151,7 @@
         <v>16.983358700718199</v>
       </c>
       <c r="L88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.5914954862110786E-2</v>
       </c>
     </row>
@@ -4152,7 +4163,7 @@
         <v>16.454258718088902</v>
       </c>
       <c r="C89">
-        <f>POWER(10, B89-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.3578574489252839E-2</v>
       </c>
       <c r="D89">
@@ -4162,7 +4173,7 @@
         <v>15.6998485988595</v>
       </c>
       <c r="F89">
-        <f>POWER(10, E89-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.3902540341704552E-3</v>
       </c>
       <c r="G89">
@@ -4172,7 +4183,7 @@
         <v>16.909148136977599</v>
       </c>
       <c r="I89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.8702908032766957E-2</v>
       </c>
       <c r="J89">
@@ -4182,7 +4193,7 @@
         <v>17.0135559953548</v>
       </c>
       <c r="L89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.9221116002620247E-2</v>
       </c>
     </row>
@@ -4194,7 +4205,7 @@
         <v>16.498735723914798</v>
       </c>
       <c r="C90">
-        <f>POWER(10, B90-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.5042886714066523E-2</v>
       </c>
       <c r="D90">
@@ -4204,7 +4215,7 @@
         <v>15.728178492282501</v>
       </c>
       <c r="F90">
-        <f>POWER(10, E90-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.5513729882230313E-3</v>
       </c>
       <c r="G90">
@@ -4214,7 +4225,7 @@
         <v>16.936533571861901</v>
       </c>
       <c r="I90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.1221997522015642E-2</v>
       </c>
       <c r="J90">
@@ -4224,7 +4235,7 @@
         <v>17.044256433327799</v>
       </c>
       <c r="L90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5.2826506896448265E-2</v>
       </c>
     </row>
@@ -4236,7 +4247,7 @@
         <v>16.5415880559902</v>
       </c>
       <c r="C91">
-        <f>POWER(10, B91-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.6602883364189917E-2</v>
       </c>
       <c r="D91">
@@ -4246,7 +4257,7 @@
         <v>15.756975011949599</v>
       </c>
       <c r="F91">
-        <f>POWER(10, E91-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.7262800963485266E-3</v>
       </c>
       <c r="G91">
@@ -4256,7 +4267,7 @@
         <v>16.96396335919</v>
       </c>
       <c r="I91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.390953320141875E-2</v>
       </c>
       <c r="J91">
@@ -4266,7 +4277,7 @@
         <v>17.074562007298798</v>
       </c>
       <c r="L91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5.6644463564691862E-2</v>
       </c>
     </row>
@@ -4278,7 +4289,7 @@
         <v>16.586301119090901</v>
       </c>
       <c r="C92">
-        <f>POWER(10, B92-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>1.840333704798881E-2</v>
       </c>
       <c r="D92">
@@ -4288,7 +4299,7 @@
         <v>15.784991732635</v>
       </c>
       <c r="F92">
-        <f>POWER(10, E92-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>2.9079517324681909E-3</v>
       </c>
       <c r="G92">
@@ -4298,7 +4309,7 @@
         <v>16.9914375707936</v>
       </c>
       <c r="I92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.677707178704698E-2</v>
       </c>
       <c r="J92">
@@ -4308,7 +4319,7 @@
         <v>17.104921466155702</v>
       </c>
       <c r="L92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.0745893884001201E-2</v>
       </c>
     </row>
@@ -4320,7 +4331,7 @@
         <v>16.629819408066801</v>
       </c>
       <c r="C93">
-        <f>POWER(10, B93-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.0342993908765709E-2</v>
       </c>
       <c r="D93">
@@ -4330,7 +4341,7 @@
         <v>15.8134752642215</v>
       </c>
       <c r="F93">
-        <f>POWER(10, E93-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.105065209369132E-3</v>
       </c>
       <c r="G93">
@@ -4340,7 +4351,7 @@
         <v>17.018058722813699</v>
       </c>
       <c r="I93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.9734090901710132E-2</v>
       </c>
       <c r="J93">
@@ -4350,7 +4361,7 @@
         <v>17.135334905708699</v>
       </c>
       <c r="L93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.5152392255502165E-2</v>
       </c>
     </row>
@@ -4362,7 +4373,7 @@
         <v>16.668616112807801</v>
       </c>
       <c r="C94">
-        <f>POWER(10, B94-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.2243932770098892E-2</v>
       </c>
       <c r="D94">
@@ -4372,7 +4383,7 @@
         <v>15.842845722854801</v>
       </c>
       <c r="F94">
-        <f>POWER(10, E94-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.3223178827858943E-3</v>
       </c>
       <c r="G94">
@@ -4382,7 +4393,7 @@
         <v>17.043373229065999</v>
       </c>
       <c r="I94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.2719185278398042E-2</v>
       </c>
       <c r="J94">
@@ -4392,7 +4403,7 @@
         <v>17.166255089976001</v>
       </c>
       <c r="L94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.9960120842504941E-2</v>
       </c>
     </row>
@@ -4404,7 +4415,7 @@
         <v>16.703538608669199</v>
       </c>
       <c r="C95">
-        <f>POWER(10, B95-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.4106494977233862E-2</v>
       </c>
       <c r="D95">
@@ -4414,7 +4425,7 @@
         <v>15.8718521852793</v>
       </c>
       <c r="F95">
-        <f>POWER(10, E95-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.5517929942102157E-3</v>
       </c>
       <c r="G95">
@@ -4424,7 +4435,7 @@
         <v>17.0687253908605</v>
       </c>
       <c r="I95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.5888293864650433E-2</v>
       </c>
       <c r="J95">
@@ -4434,7 +4445,7 @@
         <v>17.196324110995398</v>
       </c>
       <c r="L95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>7.4975534752289075E-2</v>
       </c>
     </row>
@@ -4446,7 +4457,7 @@
         <v>16.7380928816237</v>
       </c>
       <c r="C96">
-        <f>POWER(10, B96-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.6102874937433844E-2</v>
       </c>
       <c r="D96">
@@ -4456,7 +4467,7 @@
         <v>15.900073163550701</v>
       </c>
       <c r="F96">
-        <f>POWER(10, E96-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>3.7902567037168943E-3</v>
       </c>
       <c r="G96">
@@ -4466,7 +4477,7 @@
         <v>17.09411526421</v>
       </c>
       <c r="I96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.9253052047421151E-2</v>
       </c>
       <c r="J96">
@@ -4476,7 +4487,7 @@
         <v>17.2273543484059</v>
       </c>
       <c r="L96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.052853704923231E-2</v>
       </c>
     </row>
@@ -4488,7 +4499,7 @@
         <v>16.772718636304699</v>
       </c>
       <c r="C97">
-        <f>POWER(10, B97-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>2.8269237680855073E-2</v>
       </c>
       <c r="D97">
@@ -4498,7 +4509,7 @@
         <v>15.926664287557299</v>
       </c>
       <c r="F97">
-        <f>POWER(10, E97-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>4.0295796866212331E-3</v>
       </c>
       <c r="G97">
@@ -4508,7 +4519,7 @@
         <v>17.1195429052108</v>
       </c>
       <c r="I97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6.2825849005588144E-2</v>
       </c>
       <c r="J97">
@@ -4518,7 +4529,7 @@
         <v>17.2552551383755</v>
       </c>
       <c r="L97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.5871806508567336E-2</v>
       </c>
     </row>
@@ -4530,7 +4541,7 @@
         <v>16.8083024668063</v>
       </c>
       <c r="C98">
-        <f>POWER(10, B98-10)/$N$3</f>
+        <f t="shared" si="6"/>
         <v>3.0683007611160142E-2</v>
       </c>
       <c r="D98">
@@ -4540,7 +4551,7 @@
         <v>15.9537205762292</v>
       </c>
       <c r="F98">
-        <f>POWER(10, E98-10)/$N$3</f>
+        <f t="shared" si="7"/>
         <v>4.2886048976280775E-3</v>
       </c>
       <c r="G98">
@@ -4550,7 +4561,7 @@
         <v>17.145008370042699</v>
       </c>
       <c r="I98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6.66198776923521E-2</v>
       </c>
       <c r="J98">
@@ -4560,7 +4571,7 @@
         <v>17.282289623731501</v>
       </c>
       <c r="L98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.1387139708775364E-2</v>
       </c>
     </row>
@@ -4572,7 +4583,7 @@
         <v>16.844405970473002</v>
       </c>
       <c r="C99">
-        <f>POWER(10, B99-10)/$N$3</f>
+        <f t="shared" ref="C99:C130" si="10">POWER(10, B99-10)/$N$3</f>
         <v>3.334275117607232E-2</v>
       </c>
       <c r="D99">
@@ -4582,7 +4593,7 @@
         <v>15.9812442479691</v>
       </c>
       <c r="F99">
-        <f>POWER(10, E99-10)/$N$3</f>
+        <f t="shared" ref="F99:F130" si="11">POWER(10, E99-10)/$N$3</f>
         <v>4.5691951691627201E-3</v>
       </c>
       <c r="G99">
@@ -4592,7 +4603,7 @@
         <v>17.170058934685201</v>
       </c>
       <c r="I99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.0575570208877184E-2</v>
       </c>
       <c r="J99">
@@ -4602,7 +4613,7 @@
         <v>17.308453593445002</v>
       </c>
       <c r="L99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.7061959449020047E-2</v>
       </c>
     </row>
@@ -4614,7 +4625,7 @@
         <v>16.880141887824902</v>
       </c>
       <c r="C100">
-        <f>POWER(10, B100-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>3.6202398852344039E-2</v>
       </c>
       <c r="D100">
@@ -4624,7 +4635,7 @@
         <v>16.0079711216889</v>
       </c>
       <c r="F100">
-        <f>POWER(10, E100-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>4.859220230428318E-3</v>
       </c>
       <c r="G100">
@@ -4634,7 +4645,7 @@
         <v>17.1960529963361</v>
       </c>
       <c r="I100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.4928744788280127E-2</v>
       </c>
       <c r="J100">
@@ -4644,7 +4655,7 @@
         <v>17.3360285718123</v>
       </c>
       <c r="L100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.10342464355379004</v>
       </c>
     </row>
@@ -4656,7 +4667,7 @@
         <v>16.914615452263899</v>
       </c>
       <c r="C101">
-        <f>POWER(10, B101-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>3.9193217107601271E-2</v>
       </c>
       <c r="D101">
@@ -4666,7 +4677,7 @@
         <v>16.035165534774901</v>
       </c>
       <c r="F101">
-        <f>POWER(10, E101-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>5.1732205699834373E-3</v>
       </c>
       <c r="G101">
@@ -4676,7 +4687,7 @@
         <v>17.220269921557598</v>
       </c>
       <c r="I101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.9225571838671974E-2</v>
       </c>
       <c r="J101">
@@ -4686,7 +4697,7 @@
         <v>17.3622738978877</v>
       </c>
       <c r="L101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.10986752946772925</v>
       </c>
     </row>
@@ -4698,7 +4709,7 @@
         <v>16.950053342496201</v>
       </c>
       <c r="C102">
-        <f>POWER(10, B102-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>4.2525438790066275E-2</v>
       </c>
       <c r="D102">
@@ -4708,7 +4719,7 @@
         <v>16.062406145851799</v>
       </c>
       <c r="F102">
-        <f>POWER(10, E102-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>5.5080973433774879E-3</v>
       </c>
       <c r="G102">
@@ -4718,7 +4729,7 @@
         <v>17.246339998526299</v>
       </c>
       <c r="I102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.4127011124218221E-2</v>
       </c>
       <c r="J102">
@@ -4728,7 +4739,7 @@
         <v>17.389017499438602</v>
       </c>
       <c r="L102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.11684576073326353</v>
       </c>
     </row>
@@ -4740,7 +4751,7 @@
         <v>16.9855654788186</v>
       </c>
       <c r="C103">
-        <f>POWER(10, B103-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>4.614885602022685E-2</v>
       </c>
       <c r="D103">
@@ -4750,7 +4761,7 @@
         <v>16.089693033400899</v>
       </c>
       <c r="F103">
-        <f>POWER(10, E103-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>5.8652765541680734E-3</v>
       </c>
       <c r="G103">
@@ -4760,7 +4771,7 @@
         <v>17.270627742125299</v>
       </c>
       <c r="I103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.8965823504229755E-2</v>
       </c>
       <c r="J103">
@@ -4770,7 +4781,7 @@
         <v>17.417639410059198</v>
       </c>
       <c r="L103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.12480582948899949</v>
       </c>
     </row>
@@ -4782,7 +4793,7 @@
         <v>17.0220497357361</v>
       </c>
       <c r="C104">
-        <f>POWER(10, B104-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>5.019323609392564E-2</v>
       </c>
       <c r="D104">
@@ -4792,7 +4803,7 @@
         <v>16.116601275789399</v>
       </c>
       <c r="F104">
-        <f>POWER(10, E104-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>6.240174533529136E-3</v>
       </c>
       <c r="G104">
@@ -4802,7 +4813,7 @@
         <v>17.296774056706099</v>
       </c>
       <c r="I104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.4486446846763023E-2</v>
       </c>
       <c r="J104">
@@ -4812,7 +4823,7 @@
         <v>17.4444682926745</v>
       </c>
       <c r="L104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.13275893312014883</v>
       </c>
     </row>
@@ -4824,7 +4835,7 @@
         <v>17.058612359252798</v>
       </c>
       <c r="C105">
-        <f>POWER(10, B105-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>5.4601908170891979E-2</v>
       </c>
       <c r="D105">
@@ -4834,7 +4845,7 @@
         <v>16.1444059525078</v>
       </c>
       <c r="F105">
-        <f>POWER(10, E105-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>6.6527532146996322E-3</v>
       </c>
       <c r="G105">
@@ -4844,7 +4855,7 @@
         <v>17.321132825779099</v>
       </c>
       <c r="I105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.9937455283989965E-2</v>
       </c>
       <c r="J105">
@@ -4854,7 +4865,7 @@
         <v>17.474563831622302</v>
       </c>
       <c r="L105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.14228505713819584</v>
       </c>
     </row>
@@ -4866,7 +4877,7 @@
         <v>17.092999657808701</v>
       </c>
       <c r="C106">
-        <f>POWER(10, B106-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>5.910103939824693E-2</v>
       </c>
       <c r="D106">
@@ -4876,7 +4887,7 @@
         <v>16.171832141695901</v>
       </c>
       <c r="F106">
-        <f>POWER(10, E106-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>7.0864316509780872E-3</v>
       </c>
       <c r="G106">
@@ -4886,7 +4897,7 @@
         <v>17.347355600916199</v>
       </c>
       <c r="I106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.10615759277052153</v>
       </c>
       <c r="J106">
@@ -4896,7 +4907,7 @@
         <v>17.499172979179502</v>
       </c>
       <c r="L106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.15058039781880431</v>
       </c>
     </row>
@@ -4908,7 +4919,7 @@
         <v>17.129262974196301</v>
       </c>
       <c r="C107">
-        <f>POWER(10, B107-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>6.4247825773706885E-2</v>
       </c>
       <c r="D107">
@@ -4918,7 +4929,7 @@
         <v>16.196314969815301</v>
       </c>
       <c r="F107">
-        <f>POWER(10, E107-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>7.4973956657973474E-3</v>
       </c>
       <c r="G107">
@@ -4928,7 +4939,7 @@
         <v>17.371785603165399</v>
       </c>
       <c r="I107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.11230033819626797</v>
       </c>
       <c r="J107">
@@ -4938,7 +4949,7 @@
         <v>17.524278892402101</v>
       </c>
       <c r="L107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.15954175070230611</v>
       </c>
     </row>
@@ -4950,7 +4961,7 @@
         <v>17.164697934547199</v>
       </c>
       <c r="C108">
-        <f>POWER(10, B108-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>6.9709729182843239E-2</v>
       </c>
       <c r="D108">
@@ -4960,7 +4971,7 @@
         <v>16.219979398923002</v>
       </c>
       <c r="F108">
-        <f>POWER(10, E108-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>7.9172591370473347E-3</v>
       </c>
       <c r="G108">
@@ -4970,7 +4981,7 @@
         <v>17.397626281143399</v>
       </c>
       <c r="I108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.11918503878293335</v>
       </c>
       <c r="J108">
@@ -4980,7 +4991,7 @@
         <v>17.551734867830501</v>
       </c>
       <c r="L108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.16995358453036502</v>
       </c>
     </row>
@@ -4992,7 +5003,7 @@
         <v>17.201566960199401</v>
       </c>
       <c r="C109">
-        <f>POWER(10, B109-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>7.5886132745941567E-2</v>
       </c>
       <c r="D109">
@@ -5002,7 +5013,7 @@
         <v>16.2441067554326</v>
       </c>
       <c r="F109">
-        <f>POWER(10, E109-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>8.3695520856360544E-3</v>
       </c>
       <c r="G109">
@@ -5012,7 +5023,7 @@
         <v>17.4225865061901</v>
       </c>
       <c r="I109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.12623563446911712</v>
       </c>
       <c r="J109">
@@ -5022,7 +5033,7 @@
         <v>17.5773797003909</v>
       </c>
       <c r="L109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.18029146237555993</v>
       </c>
     </row>
@@ -5034,7 +5045,7 @@
         <v>17.2385151789173</v>
       </c>
       <c r="C110">
-        <f>POWER(10, B110-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>8.2624841599784907E-2</v>
       </c>
       <c r="D110">
@@ -5044,7 +5055,7 @@
         <v>16.268270001589102</v>
       </c>
       <c r="F110">
-        <f>POWER(10, E110-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>8.8484145776810512E-3</v>
       </c>
       <c r="G110">
@@ -5054,7 +5065,7 @@
         <v>17.4485027509409</v>
       </c>
       <c r="I110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.13399796779509332</v>
       </c>
       <c r="J110">
@@ -5064,7 +5075,7 @@
         <v>17.6058473785566</v>
       </c>
       <c r="L110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.1925053658987923</v>
       </c>
     </row>
@@ -5076,7 +5087,7 @@
         <v>17.273720633219799</v>
       </c>
       <c r="C111">
-        <f>POWER(10, B111-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>8.9601667951801592E-2</v>
       </c>
       <c r="D111">
@@ -5086,7 +5097,7 @@
         <v>16.292469190778501</v>
       </c>
       <c r="F111">
-        <f>POWER(10, E111-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>9.3554493480074736E-3</v>
       </c>
       <c r="G111">
@@ -5096,7 +5107,7 @@
         <v>17.473535968022102</v>
       </c>
       <c r="I111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.14194870310665331</v>
       </c>
       <c r="J111">
@@ -5106,7 +5117,7 @@
         <v>17.6329661632289</v>
       </c>
       <c r="L111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.20490927853694554</v>
       </c>
     </row>
@@ -5118,7 +5129,7 @@
         <v>17.310367354629399</v>
       </c>
       <c r="C112">
-        <f>POWER(10, B112-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>9.7490616248402995E-2</v>
       </c>
       <c r="D112">
@@ -5128,7 +5139,7 @@
         <v>16.3162741107787</v>
       </c>
       <c r="F112">
-        <f>POWER(10, E112-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>9.8825625489176623E-3</v>
       </c>
       <c r="G112">
@@ -5138,7 +5149,7 @@
         <v>17.500912442519599</v>
       </c>
       <c r="I112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.15118472124690049</v>
       </c>
       <c r="J112">
@@ -5148,7 +5159,7 @@
         <v>17.660126719732201</v>
       </c>
       <c r="L112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.21813340605165038</v>
       </c>
     </row>
@@ -5160,7 +5171,7 @@
         <v>17.343432667793699</v>
       </c>
       <c r="C113">
-        <f>POWER(10, B113-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.10520300104634855</v>
       </c>
       <c r="D113">
@@ -5170,7 +5181,7 @@
         <v>16.3409756121981</v>
       </c>
       <c r="F113">
-        <f>POWER(10, E113-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.046094872041365E-2</v>
       </c>
       <c r="G113">
@@ -5180,7 +5191,7 @@
         <v>17.524634423096799</v>
       </c>
       <c r="I113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.15967241138439525</v>
       </c>
       <c r="J113">
@@ -5190,7 +5201,7 @@
         <v>17.6887284119295</v>
       </c>
       <c r="L113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.23298280675096639</v>
       </c>
     </row>
@@ -5202,7 +5213,7 @@
         <v>17.370605304345201</v>
       </c>
       <c r="C114">
-        <f>POWER(10, B114-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.11199554960255048</v>
       </c>
       <c r="D114">
@@ -5212,7 +5223,7 @@
         <v>16.364851404910599</v>
       </c>
       <c r="F114">
-        <f>POWER(10, E114-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.1052152426855194E-2</v>
       </c>
       <c r="G114">
@@ -5222,7 +5233,7 @@
         <v>17.5497768656343</v>
       </c>
       <c r="I114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.16918907912775349</v>
       </c>
       <c r="J114">
@@ -5232,7 +5243,7 @@
         <v>17.715974860601602</v>
       </c>
       <c r="L114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.24806775800851075</v>
       </c>
     </row>
@@ -5244,7 +5255,7 @@
         <v>17.3969029767592</v>
       </c>
       <c r="C115">
-        <f>POWER(10, B115-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.11898670489457835</v>
       </c>
       <c r="D115">
@@ -5254,7 +5265,7 @@
         <v>16.389194259754099</v>
       </c>
       <c r="F115">
-        <f>POWER(10, E115-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.1689332729937928E-2</v>
       </c>
       <c r="G115">
@@ -5264,7 +5275,7 @@
         <v>17.574955379818199</v>
       </c>
       <c r="I115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17928784239106191</v>
       </c>
       <c r="J115">
@@ -5274,7 +5285,7 @@
         <v>17.702992432412099</v>
       </c>
       <c r="L115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.24076197287364265</v>
       </c>
     </row>
@@ -5286,7 +5297,7 @@
         <v>17.4236999184597</v>
       </c>
       <c r="C116">
-        <f>POWER(10, B116-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.12655968331855597</v>
       </c>
       <c r="D116">
@@ -5296,7 +5307,7 @@
         <v>16.414871853545598</v>
       </c>
       <c r="F116">
-        <f>POWER(10, E116-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.2401302880843392E-2</v>
       </c>
       <c r="G116">
@@ -5306,7 +5317,7 @@
         <v>17.591124237289499</v>
       </c>
       <c r="I116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.18608856988178557</v>
       </c>
     </row>
@@ -5318,7 +5329,7 @@
         <v>17.450538136247498</v>
       </c>
       <c r="C117">
-        <f>POWER(10, B117-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.13462744299695942</v>
       </c>
       <c r="D117">
@@ -5328,7 +5339,7 @@
         <v>16.441890343523902</v>
       </c>
       <c r="F117">
-        <f>POWER(10, E117-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.3197321738226667E-2</v>
       </c>
     </row>
@@ -5340,7 +5351,7 @@
         <v>17.476956820416198</v>
       </c>
       <c r="C118">
-        <f>POWER(10, B118-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.14307122030048897</v>
       </c>
       <c r="D118">
@@ -5350,7 +5361,7 @@
         <v>16.468519024858299</v>
       </c>
       <c r="F118">
-        <f>POWER(10, E118-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.4031835538111742E-2</v>
       </c>
     </row>
@@ -5362,7 +5373,7 @@
         <v>17.5038770713163</v>
       </c>
       <c r="C119">
-        <f>POWER(10, B119-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.15222028555273115</v>
       </c>
       <c r="D119">
@@ -5372,7 +5383,7 @@
         <v>16.496060812062201</v>
       </c>
       <c r="F119">
-        <f>POWER(10, E119-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.495051913111653E-2</v>
       </c>
     </row>
@@ -5384,7 +5395,7 @@
         <v>17.530376506260001</v>
       </c>
       <c r="C120">
-        <f>POWER(10, B120-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.16179755975217205</v>
       </c>
       <c r="D120">
@@ -5394,7 +5405,7 @@
         <v>16.522777225896601</v>
       </c>
       <c r="F120">
-        <f>POWER(10, E120-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.5899105343784057E-2</v>
       </c>
     </row>
@@ -5406,7 +5417,7 @@
         <v>17.557842035059402</v>
       </c>
       <c r="C121">
-        <f>POWER(10, B121-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.17236040109423761</v>
       </c>
       <c r="D121">
@@ -5416,7 +5427,7 @@
         <v>16.550409753975501</v>
       </c>
       <c r="F121">
-        <f>POWER(10, E121-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.6943581460136036E-2</v>
       </c>
     </row>
@@ -5428,7 +5439,7 @@
         <v>17.583959473553001</v>
       </c>
       <c r="C122">
-        <f>POWER(10, B122-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.18304376263978656</v>
       </c>
       <c r="D122">
@@ -5438,7 +5449,7 @@
         <v>16.577214189358799</v>
       </c>
       <c r="F122">
-        <f>POWER(10, E122-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.80222765807036E-2</v>
       </c>
     </row>
@@ -5450,7 +5461,7 @@
         <v>17.611508952889899</v>
       </c>
       <c r="C123">
-        <f>POWER(10, B123-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.19503134413510831</v>
       </c>
       <c r="D123">
@@ -5460,7 +5471,7 @@
         <v>16.604062036220601</v>
       </c>
       <c r="F123">
-        <f>POWER(10, E123-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>1.9171561947773894E-2</v>
       </c>
     </row>
@@ -5472,7 +5483,7 @@
         <v>17.637706221377599</v>
       </c>
       <c r="C124">
-        <f>POWER(10, B124-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.2071579870655274</v>
       </c>
       <c r="D124">
@@ -5482,7 +5493,7 @@
         <v>16.623937915284699</v>
       </c>
       <c r="F124">
-        <f>POWER(10, E124-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.0069353205106527E-2</v>
       </c>
     </row>
@@ -5494,7 +5505,7 @@
         <v>17.6653399078535</v>
       </c>
       <c r="C125">
-        <f>POWER(10, B125-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.22076761649940962</v>
       </c>
       <c r="D125">
@@ -5504,7 +5515,7 @@
         <v>16.6433986946797</v>
       </c>
       <c r="F125">
-        <f>POWER(10, E125-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.098911638239867E-2</v>
       </c>
     </row>
@@ -5516,7 +5527,7 @@
         <v>17.692083784295299</v>
       </c>
       <c r="C126">
-        <f>POWER(10, B126-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.23478981049083331</v>
       </c>
       <c r="D126">
@@ -5526,7 +5537,7 @@
         <v>16.661564107730499</v>
       </c>
       <c r="F126">
-        <f>POWER(10, E126-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.1885656002367367E-2</v>
       </c>
     </row>
@@ -5538,7 +5549,7 @@
         <v>17.719335401342398</v>
       </c>
       <c r="C127">
-        <f>POWER(10, B127-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.24999473499943231</v>
       </c>
       <c r="D127">
@@ -5548,7 +5559,7 @@
         <v>16.6793095083402</v>
       </c>
       <c r="F127">
-        <f>POWER(10, E127-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.2798431507960952E-2</v>
       </c>
     </row>
@@ -5560,7 +5571,7 @@
         <v>17.7461610225348</v>
       </c>
       <c r="C128">
-        <f>POWER(10, B128-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.2659233563142549</v>
       </c>
       <c r="D128">
@@ -5570,7 +5581,7 @@
         <v>16.6970738086907</v>
       </c>
       <c r="F128">
-        <f>POWER(10, E128-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.3750309292977379E-2</v>
       </c>
     </row>
@@ -5582,7 +5593,7 @@
         <v>17.773964629403601</v>
       </c>
       <c r="C129">
-        <f>POWER(10, B129-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.28350458725022554</v>
       </c>
       <c r="D129">
@@ -5592,7 +5603,7 @@
         <v>16.7152978053659</v>
       </c>
       <c r="F129">
-        <f>POWER(10, E129-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.4768132730329701E-2</v>
       </c>
     </row>
@@ -5604,7 +5615,7 @@
         <v>17.8004035520839</v>
       </c>
       <c r="C130">
-        <f>POWER(10, B130-10)/$N$3</f>
+        <f t="shared" si="10"/>
         <v>0.30129991771978143</v>
       </c>
       <c r="D130">
@@ -5614,7 +5625,7 @@
         <v>16.734865535031901</v>
       </c>
       <c r="F130">
-        <f>POWER(10, E130-10)/$N$3</f>
+        <f t="shared" si="11"/>
         <v>2.5909617166923485E-2</v>
       </c>
     </row>
@@ -5626,7 +5637,7 @@
         <v>17.828292142852298</v>
       </c>
       <c r="C131">
-        <f>POWER(10, B131-10)/$N$3</f>
+        <f t="shared" ref="C131:C162" si="12">POWER(10, B131-10)/$N$3</f>
         <v>0.32128289453919295</v>
       </c>
       <c r="D131">
@@ -5636,7 +5647,7 @@
         <v>16.761084705575101</v>
       </c>
       <c r="F131">
-        <f>POWER(10, E131-10)/$N$3</f>
+        <f t="shared" ref="F131:F162" si="13">POWER(10, E131-10)/$N$3</f>
         <v>2.7522011156600055E-2</v>
       </c>
     </row>
@@ -5648,7 +5659,7 @@
         <v>17.854811878168199</v>
       </c>
       <c r="C132">
-        <f>POWER(10, B132-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.3415130778623866</v>
       </c>
       <c r="D132">
@@ -5658,7 +5669,7 @@
         <v>16.788673053701402</v>
       </c>
       <c r="F132">
-        <f>POWER(10, E132-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>2.932705912158317E-2</v>
       </c>
     </row>
@@ -5670,7 +5681,7 @@
         <v>17.8827857125961</v>
       </c>
       <c r="C133">
-        <f>POWER(10, B133-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.36423457896525047</v>
       </c>
       <c r="D133">
@@ -5680,7 +5691,7 @@
         <v>16.8163068115946</v>
       </c>
       <c r="F133">
-        <f>POWER(10, E133-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.1253759981027626E-2</v>
       </c>
     </row>
@@ -5692,7 +5703,7 @@
         <v>17.909858784160399</v>
       </c>
       <c r="C134">
-        <f>POWER(10, B134-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.38766290435324507</v>
       </c>
       <c r="D134">
@@ -5702,7 +5713,7 @@
         <v>16.843541884080398</v>
       </c>
       <c r="F134">
-        <f>POWER(10, E134-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.3276477308652588E-2</v>
       </c>
     </row>
@@ -5714,7 +5725,7 @@
         <v>17.937445846199299</v>
       </c>
       <c r="C135">
-        <f>POWER(10, B135-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.41308679017760908</v>
       </c>
       <c r="D135">
@@ -5724,7 +5735,7 @@
         <v>16.869486468038801</v>
       </c>
       <c r="F135">
-        <f>POWER(10, E135-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.5324980357393149E-2</v>
       </c>
     </row>
@@ -5736,7 +5747,7 @@
         <v>17.964601668724899</v>
       </c>
       <c r="C136">
-        <f>POWER(10, B136-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.43974117215563574</v>
       </c>
       <c r="D136">
@@ -5746,7 +5757,7 @@
         <v>16.8972532428965</v>
       </c>
       <c r="F136">
-        <f>POWER(10, E136-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.765725887187199E-2</v>
       </c>
     </row>
@@ -5758,7 +5769,7 @@
         <v>17.992273052777101</v>
       </c>
       <c r="C137">
-        <f>POWER(10, B137-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.46867146651563363</v>
       </c>
       <c r="D137">
@@ -5768,7 +5779,7 @@
         <v>16.917514761469299</v>
       </c>
       <c r="F137">
-        <f>POWER(10, E137-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>3.945574266997235E-2</v>
       </c>
     </row>
@@ -5780,7 +5791,7 @@
         <v>18.019987059844901</v>
       </c>
       <c r="C138">
-        <f>POWER(10, B138-10)/$N$3</f>
+        <f t="shared" si="12"/>
         <v>0.49955409208607204</v>
       </c>
       <c r="D138">
@@ -5790,7 +5801,7 @@
         <v>16.691477043366401</v>
       </c>
       <c r="F138">
-        <f>POWER(10, E138-10)/$N$3</f>
+        <f t="shared" si="13"/>
         <v>2.3446202110167215E-2</v>
       </c>
     </row>

</xml_diff>